<commit_message>
added conditional colouring to tables
</commit_message>
<xml_diff>
--- a/xlsx_data/codewars_stats_Filpill.xlsx
+++ b/xlsx_data/codewars_stats_Filpill.xlsx
@@ -22,7 +22,7 @@
     <t>4 kyu</t>
   </si>
   <si>
-    <t>Filpill Codewars Stats since 11-Nov-2022</t>
+    <t>Filpill Codewars Stats since 12-Nov-2022</t>
   </si>
   <si>
     <t>Username</t>
@@ -736,7 +736,7 @@
     <t>white</t>
   </si>
   <si>
-    <t>Kata Compeleted By Filpill since 11-Nov-2022</t>
+    <t>Kata Compeleted By Filpill since 12-Nov-2022</t>
   </si>
   <si>
     <t>Kata ID</t>
@@ -838,7 +838,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0E0DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B831"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3B7EBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF856DCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -4312,6 +4353,82 @@
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B8:L8"/>
   </mergeCells>
+  <conditionalFormatting sqref="H4:I4">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="white">
+      <formula>NOT(ISERROR(SEARCH("white",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="8 kyu">
+      <formula>NOT(ISERROR(SEARCH("8 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="7 kyu">
+      <formula>NOT(ISERROR(SEARCH("7 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="yellow">
+      <formula>NOT(ISERROR(SEARCH("yellow",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="6 kyu">
+      <formula>NOT(ISERROR(SEARCH("6 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="5 kyu">
+      <formula>NOT(ISERROR(SEARCH("5 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="blue">
+      <formula>NOT(ISERROR(SEARCH("blue",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="4 kyu">
+      <formula>NOT(ISERROR(SEARCH("4 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="3 kyu">
+      <formula>NOT(ISERROR(SEARCH("3 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="purple">
+      <formula>NOT(ISERROR(SEARCH("purple",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="2 kyu">
+      <formula>NOT(ISERROR(SEARCH("2 kyu",H4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="1 kyu">
+      <formula>NOT(ISERROR(SEARCH("1 kyu",H4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10:L95">
+    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="white">
+      <formula>NOT(ISERROR(SEARCH("white",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="14" operator="containsText" text="8 kyu">
+      <formula>NOT(ISERROR(SEARCH("8 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="15" operator="containsText" text="7 kyu">
+      <formula>NOT(ISERROR(SEARCH("7 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="16" operator="containsText" text="yellow">
+      <formula>NOT(ISERROR(SEARCH("yellow",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="6 kyu">
+      <formula>NOT(ISERROR(SEARCH("6 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="18" operator="containsText" text="5 kyu">
+      <formula>NOT(ISERROR(SEARCH("5 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="19" operator="containsText" text="blue">
+      <formula>NOT(ISERROR(SEARCH("blue",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="4 kyu">
+      <formula>NOT(ISERROR(SEARCH("4 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="21" operator="containsText" text="3 kyu">
+      <formula>NOT(ISERROR(SEARCH("3 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="22" operator="containsText" text="purple">
+      <formula>NOT(ISERROR(SEARCH("purple",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="23" operator="containsText" text="2 kyu">
+      <formula>NOT(ISERROR(SEARCH("2 kyu",K10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="24" operator="containsText" text="1 kyu">
+      <formula>NOT(ISERROR(SEARCH("1 kyu",K10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
aggregated data into each catagory
</commit_message>
<xml_diff>
--- a/xlsx_data/codewars_stats_Filpill.xlsx
+++ b/xlsx_data/codewars_stats_Filpill.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="252">
   <si>
     <t>Filpill</t>
   </si>
@@ -46,718 +46,721 @@
     <t>SQL Score</t>
   </si>
   <si>
+    <t>codeChallenges.totalCompleted</t>
+  </si>
+  <si>
+    <t>5324945e2ece5e1f32000370</t>
+  </si>
+  <si>
+    <t>521c2db8ddc89b9b7a0000c1</t>
+  </si>
+  <si>
+    <t>546d15cebed2e10334000ed9</t>
+  </si>
+  <si>
+    <t>55c6126177c9441a570000cc</t>
+  </si>
+  <si>
+    <t>52bc74d4ac05d0945d00054e</t>
+  </si>
+  <si>
+    <t>5541f58a944b85ce6d00006a</t>
+  </si>
+  <si>
+    <t>525c65e51bf619685c000059</t>
+  </si>
+  <si>
+    <t>514a024011ea4fb54200004b</t>
+  </si>
+  <si>
+    <t>525f3eda17c7cd9f9e000b39</t>
+  </si>
+  <si>
+    <t>52449b062fb80683ec000024</t>
+  </si>
+  <si>
+    <t>530e15517bc88ac656000716</t>
+  </si>
+  <si>
+    <t>513e08acc600c94f01000001</t>
+  </si>
+  <si>
+    <t>52774a314c2333f0a7000688</t>
+  </si>
+  <si>
+    <t>52597aa56021e91c93000cb0</t>
+  </si>
+  <si>
+    <t>520b9d2ad5c005041100000f</t>
+  </si>
+  <si>
+    <t>522551eee9abb932420004a0</t>
+  </si>
+  <si>
+    <t>54bf1c2cd5b56cc47f0007a1</t>
+  </si>
+  <si>
+    <t>526571aae218b8ee490006f4</t>
+  </si>
+  <si>
+    <t>5264d2b162488dc400000001</t>
+  </si>
+  <si>
+    <t>541c8630095125aba6000c00</t>
+  </si>
+  <si>
+    <t>54da5a58ea159efa38000836</t>
+  </si>
+  <si>
+    <t>5266876b8f4bf2da9b000362</t>
+  </si>
+  <si>
+    <t>514b92a657cdc65150000006</t>
+  </si>
+  <si>
+    <t>582001237a3a630ce8000a41</t>
+  </si>
+  <si>
+    <t>5812a2a2492760dfca000450</t>
+  </si>
+  <si>
+    <t>589cf45835f99b2909000115</t>
+  </si>
+  <si>
+    <t>5817b124e7f4576fd00020a2</t>
+  </si>
+  <si>
+    <t>59be9f425227ddd60c00003b</t>
+  </si>
+  <si>
+    <t>5982020284a83baf2f00001c</t>
+  </si>
+  <si>
+    <t>594257d4db68b6e99200002c</t>
+  </si>
+  <si>
+    <t>5811010104adbba24b0002fe</t>
+  </si>
+  <si>
+    <t>581676828906324b8b00059e</t>
+  </si>
+  <si>
+    <t>5816a3ecf54413a113000074</t>
+  </si>
+  <si>
+    <t>582cba7d3be8ce3a8300007c</t>
+  </si>
+  <si>
+    <t>5811501c2d35672d4f000146</t>
+  </si>
+  <si>
+    <t>593ef0e98b90525e090000b9</t>
+  </si>
+  <si>
+    <t>5dac87a0abe9f1001f39e36d</t>
+  </si>
+  <si>
+    <t>58112f8004adbbdb500004fe</t>
+  </si>
+  <si>
+    <t>5db039743affec0027375de0</t>
+  </si>
+  <si>
+    <t>5994dafcbddc2f116d000024</t>
+  </si>
+  <si>
+    <t>580d08b5c049aef8f900007c</t>
+  </si>
+  <si>
+    <t>58094559c47d323ebd000035</t>
+  </si>
+  <si>
+    <t>58113a64e10b53ec36000293</t>
+  </si>
+  <si>
+    <t>58164ddf890632ce00000220</t>
+  </si>
+  <si>
+    <t>5811315e04adbbdb5000050e</t>
+  </si>
+  <si>
+    <t>5818bde9559ff58bd90004a2</t>
+  </si>
+  <si>
+    <t>5e5f09dc0a17be0023920f6f</t>
+  </si>
+  <si>
+    <t>58126aa90ea99769e7000119</t>
+  </si>
+  <si>
+    <t>5daf515c3affec002b2fb921</t>
+  </si>
+  <si>
+    <t>58241d05e7a162c5b100010f</t>
+  </si>
+  <si>
+    <t>58167fa1f544130dcf000317</t>
+  </si>
+  <si>
+    <t>5811597e9d278beb04000038</t>
+  </si>
+  <si>
+    <t>526989a41034285187000de4</t>
+  </si>
+  <si>
+    <t>594323fde53209e94700012a</t>
+  </si>
+  <si>
+    <t>5820176255c3d23f360000a9</t>
+  </si>
+  <si>
+    <t>5811527d9d278b242f000006</t>
+  </si>
+  <si>
+    <t>5809575e166583acfa000083</t>
+  </si>
+  <si>
+    <t>5a8ed96bfd8c066e7f00011a</t>
+  </si>
+  <si>
+    <t>59401c25c15cbeb58d000028</t>
+  </si>
+  <si>
+    <t>58113c03009b4fcc66000d29</t>
+  </si>
+  <si>
+    <t>520446778469526ec0000001</t>
+  </si>
+  <si>
+    <t>580fb94e12b34dd1c40001f0</t>
+  </si>
+  <si>
+    <t>580918e24a85b05ad000010c</t>
+  </si>
+  <si>
+    <t>5629db57620258aa9d000014</t>
+  </si>
+  <si>
+    <t>559a28007caad2ac4e000083</t>
+  </si>
+  <si>
+    <t>550f22f4d758534c1100025a</t>
+  </si>
+  <si>
+    <t>52efefcbcdf57161d4000091</t>
+  </si>
+  <si>
+    <t>54a91a4883a7de5d7800009c</t>
+  </si>
+  <si>
+    <t>52742f58faf5485cae000b9a</t>
+  </si>
+  <si>
+    <t>52685f7382004e774f0001f7</t>
+  </si>
+  <si>
+    <t>523a86aa4230ebb5420001e1</t>
+  </si>
+  <si>
+    <t>51c8e37cee245da6b40000bd</t>
+  </si>
+  <si>
+    <t>5842df8ccbd22792a4000245</t>
+  </si>
+  <si>
+    <t>5287e858c6b5a9678200083c</t>
+  </si>
+  <si>
+    <t>523f5d21c841566fde000009</t>
+  </si>
+  <si>
+    <t>51b62bf6a9c58071c600001b</t>
+  </si>
+  <si>
+    <t>56a5d994ac971f1ac500003e</t>
+  </si>
+  <si>
+    <t>550554fd08b86f84fe000a58</t>
+  </si>
+  <si>
+    <t>54521e9ec8e60bc4de000d6c</t>
+  </si>
+  <si>
+    <t>5208f99aee097e6552000148</t>
+  </si>
+  <si>
+    <t>55fd2d567d94ac3bc9000064</t>
+  </si>
+  <si>
+    <t>55bf01e5a717a0d57e0000ec</t>
+  </si>
+  <si>
+    <t>55b42574ff091733d900002f</t>
+  </si>
+  <si>
+    <t>5552101f47fc5178b1000050</t>
+  </si>
+  <si>
+    <t>525f50e3b73515a6db000b83</t>
+  </si>
+  <si>
+    <t>50654ddff44f800200000004</t>
+  </si>
+  <si>
+    <t>Sum Strings as Numbers</t>
+  </si>
+  <si>
+    <t>Snail</t>
+  </si>
+  <si>
+    <t>Find the unknown digit</t>
+  </si>
+  <si>
+    <t>Weight for weight</t>
+  </si>
+  <si>
+    <t>First non-repeating character</t>
+  </si>
+  <si>
+    <t>Product of consecutive Fib numbers</t>
+  </si>
+  <si>
+    <t>Pete, the baker</t>
+  </si>
+  <si>
+    <t>Extract the domain name from a URL</t>
+  </si>
+  <si>
+    <t>Calculating with Functions</t>
+  </si>
+  <si>
+    <t>The Hashtag Generator</t>
+  </si>
+  <si>
+    <t>Rot13</t>
+  </si>
+  <si>
+    <t>RGB To Hex Conversion</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Moving Zeros To The End</t>
+  </si>
+  <si>
+    <t>Simple Pig Latin</t>
+  </si>
+  <si>
+    <t>N-th Fibonacci</t>
+  </si>
+  <si>
+    <t>Counting Duplicates</t>
+  </si>
+  <si>
+    <t>Bit Counting</t>
+  </si>
+  <si>
+    <t>Stop gninnipS My sdroW!</t>
+  </si>
+  <si>
+    <t>Sum of Digits / Digital Root</t>
+  </si>
+  <si>
+    <t>Find the odd int</t>
+  </si>
+  <si>
+    <t>Who likes it?</t>
+  </si>
+  <si>
+    <t>Multiples of 3 or 5</t>
+  </si>
+  <si>
+    <t>Using Window Functions To Get Top N per Group</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple Hierarchical structure</t>
+  </si>
+  <si>
+    <t>Calculating  Running Total</t>
+  </si>
+  <si>
+    <t>Relational division: Find all movies two actors cast in together</t>
+  </si>
+  <si>
+    <t>SELECT prime numbers</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple PIVOTING data WITHOUT CROSSTAB</t>
+  </si>
+  <si>
+    <t>SQL: Regex AlphaNumeric Split</t>
+  </si>
+  <si>
+    <t>SQL Basics: Create a FUNCTION (DATES)</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple FULL TEXT SEARCH</t>
+  </si>
+  <si>
+    <t>Conditional Count</t>
+  </si>
+  <si>
+    <t>SQL Bug Fixing: Fix the QUERY - Totaling</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple WITH</t>
+  </si>
+  <si>
+    <t>SQL Basics - Monsters using CASE</t>
+  </si>
+  <si>
+    <t>Analyzing the sales by product and date</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple UNION ALL</t>
+  </si>
+  <si>
+    <t>Present XML data the SQL way</t>
+  </si>
+  <si>
+    <t>Calculating Batting Average</t>
+  </si>
+  <si>
+    <t>SQL Basics: Top 10 customers by total payments amount</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple JOIN and RANK</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple EXISTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Basics: Simple HAVING </t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple NULL handling</t>
+  </si>
+  <si>
+    <t>Challenge: Two actors who cast together the most</t>
+  </si>
+  <si>
+    <t>Countries Capitals for Trivia Night (SQL for Beginners #6)</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple PIVOTING data</t>
+  </si>
+  <si>
+    <t>Present JSON data the SQL way</t>
+  </si>
+  <si>
+    <t>Count Weekdays</t>
+  </si>
+  <si>
+    <t>SQL Statistics: MIN, MEDIAN, MAX</t>
+  </si>
+  <si>
+    <t>SQL Basics: Group By Day</t>
+  </si>
+  <si>
+    <t>Count IP Addresses</t>
+  </si>
+  <si>
+    <t>Subqueries master</t>
+  </si>
+  <si>
+    <t>Using LATERAL JOIN To Get Top N per Group</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple VIEW</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple table totaling.</t>
+  </si>
+  <si>
+    <t>GROCERY STORE: Support Local Products</t>
+  </si>
+  <si>
+    <t>SQL Basics - Trimming the Field</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple IN</t>
+  </si>
+  <si>
+    <t>Nesting Structure Comparison</t>
+  </si>
+  <si>
+    <t>SQL Bug Fixing: Fix the JOIN</t>
+  </si>
+  <si>
+    <t>SQL Basics: Simple JOIN with COUNT</t>
+  </si>
+  <si>
+    <t>Strings Mix</t>
+  </si>
+  <si>
+    <t>Perimeter of squares in a rectangle</t>
+  </si>
+  <si>
+    <t>Directions Reduction</t>
+  </si>
+  <si>
+    <t>Count characters in your string</t>
+  </si>
+  <si>
+    <t>String incrementer</t>
+  </si>
+  <si>
+    <t>Human readable duration format</t>
+  </si>
+  <si>
+    <t>Human Readable Time</t>
+  </si>
+  <si>
+    <t>Where my anagrams at?</t>
+  </si>
+  <si>
+    <t>Strip Comments</t>
+  </si>
+  <si>
+    <t>Write Number in Expanded Form</t>
+  </si>
+  <si>
+    <t>Does my number look big in this?</t>
+  </si>
+  <si>
+    <t>Array.diff</t>
+  </si>
+  <si>
+    <t>Roman Numerals Encoder</t>
+  </si>
+  <si>
+    <t>Consecutive strings</t>
+  </si>
+  <si>
+    <t>Which are  in?</t>
+  </si>
+  <si>
+    <t>Maximum  subarray sum</t>
+  </si>
+  <si>
+    <t>Break camelCase</t>
+  </si>
+  <si>
+    <t>Sum of odd numbers</t>
+  </si>
+  <si>
+    <t>Persistent Bugger.</t>
+  </si>
+  <si>
+    <t>Friend or Foe?</t>
+  </si>
+  <si>
+    <t>Playing with digits</t>
+  </si>
+  <si>
+    <t>Create Phone Number</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>['python']</t>
+  </si>
+  <si>
+    <t>['sql']</t>
+  </si>
+  <si>
+    <t>Nov-22</t>
+  </si>
+  <si>
+    <t>Oct-22</t>
+  </si>
+  <si>
+    <t>Sep-22</t>
+  </si>
+  <si>
+    <t>Jun-22</t>
+  </si>
+  <si>
+    <t>algorithms</t>
+  </si>
+  <si>
+    <t>games</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>refactoring</t>
+  </si>
+  <si>
+    <t>bug_fixes</t>
+  </si>
+  <si>
+    <t>['Strings', 'Big Integers', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Arrays', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Mathematics', 'Algorithms', 'Puzzles']</t>
+  </si>
+  <si>
+    <t>['Algorithms']</t>
+  </si>
+  <si>
+    <t>['Strings', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Algorithms', 'Mathematics']</t>
+  </si>
+  <si>
+    <t>['Parsing', 'Regular Expressions']</t>
+  </si>
+  <si>
+    <t>['Functional Programming']</t>
+  </si>
+  <si>
+    <t>['Ciphers', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Arrays', 'Sorting', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Regular Expressions', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Strings', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Bits', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Mathematics', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Fundamentals']</t>
+  </si>
+  <si>
+    <t>['SQL', 'Fundamentals', 'Databases']</t>
+  </si>
+  <si>
+    <t>['SQL', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'Databases', 'SQL']</t>
+  </si>
+  <si>
+    <t>['Mathematics', 'Databases']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'SQL', 'Databases']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'Regular Expressions', 'SQL']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'SQL', 'Data Science']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'SQL']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'SQL', 'Databases', 'Data Science']</t>
+  </si>
+  <si>
+    <t>['SQL', 'Data Science', 'JSON']</t>
+  </si>
+  <si>
+    <t>['SQL', 'Statistics', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['SQL', 'Databases', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'Strings']</t>
+  </si>
+  <si>
+    <t>['Regular Expressions', 'Strings']</t>
+  </si>
+  <si>
+    <t>['Strings', 'Date Time', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Date Time', 'Mathematics', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Strings', 'Mathematics', 'Algorithms', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Arrays', 'Fundamentals', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Arrays', 'Lists', 'Strings', 'Refactoring']</t>
+  </si>
+  <si>
+    <t>['Algorithms', 'Lists', 'Dynamic Programming', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Arrays', 'Lists', 'Mathematics', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>['Fundamentals', 'Mathematics']</t>
+  </si>
+  <si>
+    <t>['Arrays', 'Strings', 'Regular Expressions', 'Algorithms']</t>
+  </si>
+  <si>
+    <t>['Debugging', 'Fundamentals']</t>
+  </si>
+  <si>
+    <t>5 kyu</t>
+  </si>
+  <si>
+    <t>6 kyu</t>
+  </si>
+  <si>
+    <t>7 kyu</t>
+  </si>
+  <si>
+    <t>8 kyu</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>Kata Compeleted By Filpill since 12-Nov-2022</t>
+  </si>
+  <si>
+    <t>Kata ID</t>
+  </si>
+  <si>
+    <t>Kata Name</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Completed Date</t>
+  </si>
+  <si>
+    <t>Completion Period</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Total Attempts</t>
+  </si>
+  <si>
     <t>Total Completed</t>
-  </si>
-  <si>
-    <t>5324945e2ece5e1f32000370</t>
-  </si>
-  <si>
-    <t>521c2db8ddc89b9b7a0000c1</t>
-  </si>
-  <si>
-    <t>546d15cebed2e10334000ed9</t>
-  </si>
-  <si>
-    <t>55c6126177c9441a570000cc</t>
-  </si>
-  <si>
-    <t>52bc74d4ac05d0945d00054e</t>
-  </si>
-  <si>
-    <t>5541f58a944b85ce6d00006a</t>
-  </si>
-  <si>
-    <t>525c65e51bf619685c000059</t>
-  </si>
-  <si>
-    <t>514a024011ea4fb54200004b</t>
-  </si>
-  <si>
-    <t>525f3eda17c7cd9f9e000b39</t>
-  </si>
-  <si>
-    <t>52449b062fb80683ec000024</t>
-  </si>
-  <si>
-    <t>530e15517bc88ac656000716</t>
-  </si>
-  <si>
-    <t>513e08acc600c94f01000001</t>
-  </si>
-  <si>
-    <t>52774a314c2333f0a7000688</t>
-  </si>
-  <si>
-    <t>52597aa56021e91c93000cb0</t>
-  </si>
-  <si>
-    <t>520b9d2ad5c005041100000f</t>
-  </si>
-  <si>
-    <t>522551eee9abb932420004a0</t>
-  </si>
-  <si>
-    <t>54bf1c2cd5b56cc47f0007a1</t>
-  </si>
-  <si>
-    <t>526571aae218b8ee490006f4</t>
-  </si>
-  <si>
-    <t>5264d2b162488dc400000001</t>
-  </si>
-  <si>
-    <t>541c8630095125aba6000c00</t>
-  </si>
-  <si>
-    <t>54da5a58ea159efa38000836</t>
-  </si>
-  <si>
-    <t>5266876b8f4bf2da9b000362</t>
-  </si>
-  <si>
-    <t>514b92a657cdc65150000006</t>
-  </si>
-  <si>
-    <t>582001237a3a630ce8000a41</t>
-  </si>
-  <si>
-    <t>5812a2a2492760dfca000450</t>
-  </si>
-  <si>
-    <t>589cf45835f99b2909000115</t>
-  </si>
-  <si>
-    <t>5817b124e7f4576fd00020a2</t>
-  </si>
-  <si>
-    <t>59be9f425227ddd60c00003b</t>
-  </si>
-  <si>
-    <t>5982020284a83baf2f00001c</t>
-  </si>
-  <si>
-    <t>594257d4db68b6e99200002c</t>
-  </si>
-  <si>
-    <t>5811010104adbba24b0002fe</t>
-  </si>
-  <si>
-    <t>581676828906324b8b00059e</t>
-  </si>
-  <si>
-    <t>5816a3ecf54413a113000074</t>
-  </si>
-  <si>
-    <t>582cba7d3be8ce3a8300007c</t>
-  </si>
-  <si>
-    <t>5811501c2d35672d4f000146</t>
-  </si>
-  <si>
-    <t>593ef0e98b90525e090000b9</t>
-  </si>
-  <si>
-    <t>5dac87a0abe9f1001f39e36d</t>
-  </si>
-  <si>
-    <t>58112f8004adbbdb500004fe</t>
-  </si>
-  <si>
-    <t>5db039743affec0027375de0</t>
-  </si>
-  <si>
-    <t>5994dafcbddc2f116d000024</t>
-  </si>
-  <si>
-    <t>580d08b5c049aef8f900007c</t>
-  </si>
-  <si>
-    <t>58094559c47d323ebd000035</t>
-  </si>
-  <si>
-    <t>58113a64e10b53ec36000293</t>
-  </si>
-  <si>
-    <t>58164ddf890632ce00000220</t>
-  </si>
-  <si>
-    <t>5811315e04adbbdb5000050e</t>
-  </si>
-  <si>
-    <t>5818bde9559ff58bd90004a2</t>
-  </si>
-  <si>
-    <t>5e5f09dc0a17be0023920f6f</t>
-  </si>
-  <si>
-    <t>58126aa90ea99769e7000119</t>
-  </si>
-  <si>
-    <t>5daf515c3affec002b2fb921</t>
-  </si>
-  <si>
-    <t>58241d05e7a162c5b100010f</t>
-  </si>
-  <si>
-    <t>58167fa1f544130dcf000317</t>
-  </si>
-  <si>
-    <t>5811597e9d278beb04000038</t>
-  </si>
-  <si>
-    <t>526989a41034285187000de4</t>
-  </si>
-  <si>
-    <t>594323fde53209e94700012a</t>
-  </si>
-  <si>
-    <t>5820176255c3d23f360000a9</t>
-  </si>
-  <si>
-    <t>5811527d9d278b242f000006</t>
-  </si>
-  <si>
-    <t>5809575e166583acfa000083</t>
-  </si>
-  <si>
-    <t>5a8ed96bfd8c066e7f00011a</t>
-  </si>
-  <si>
-    <t>59401c25c15cbeb58d000028</t>
-  </si>
-  <si>
-    <t>58113c03009b4fcc66000d29</t>
-  </si>
-  <si>
-    <t>520446778469526ec0000001</t>
-  </si>
-  <si>
-    <t>580fb94e12b34dd1c40001f0</t>
-  </si>
-  <si>
-    <t>580918e24a85b05ad000010c</t>
-  </si>
-  <si>
-    <t>5629db57620258aa9d000014</t>
-  </si>
-  <si>
-    <t>559a28007caad2ac4e000083</t>
-  </si>
-  <si>
-    <t>550f22f4d758534c1100025a</t>
-  </si>
-  <si>
-    <t>52efefcbcdf57161d4000091</t>
-  </si>
-  <si>
-    <t>54a91a4883a7de5d7800009c</t>
-  </si>
-  <si>
-    <t>52742f58faf5485cae000b9a</t>
-  </si>
-  <si>
-    <t>52685f7382004e774f0001f7</t>
-  </si>
-  <si>
-    <t>523a86aa4230ebb5420001e1</t>
-  </si>
-  <si>
-    <t>51c8e37cee245da6b40000bd</t>
-  </si>
-  <si>
-    <t>5842df8ccbd22792a4000245</t>
-  </si>
-  <si>
-    <t>5287e858c6b5a9678200083c</t>
-  </si>
-  <si>
-    <t>523f5d21c841566fde000009</t>
-  </si>
-  <si>
-    <t>51b62bf6a9c58071c600001b</t>
-  </si>
-  <si>
-    <t>56a5d994ac971f1ac500003e</t>
-  </si>
-  <si>
-    <t>550554fd08b86f84fe000a58</t>
-  </si>
-  <si>
-    <t>54521e9ec8e60bc4de000d6c</t>
-  </si>
-  <si>
-    <t>5208f99aee097e6552000148</t>
-  </si>
-  <si>
-    <t>55fd2d567d94ac3bc9000064</t>
-  </si>
-  <si>
-    <t>55bf01e5a717a0d57e0000ec</t>
-  </si>
-  <si>
-    <t>55b42574ff091733d900002f</t>
-  </si>
-  <si>
-    <t>5552101f47fc5178b1000050</t>
-  </si>
-  <si>
-    <t>525f50e3b73515a6db000b83</t>
-  </si>
-  <si>
-    <t>50654ddff44f800200000004</t>
-  </si>
-  <si>
-    <t>Sum Strings as Numbers</t>
-  </si>
-  <si>
-    <t>Snail</t>
-  </si>
-  <si>
-    <t>Find the unknown digit</t>
-  </si>
-  <si>
-    <t>Weight for weight</t>
-  </si>
-  <si>
-    <t>First non-repeating character</t>
-  </si>
-  <si>
-    <t>Product of consecutive Fib numbers</t>
-  </si>
-  <si>
-    <t>Pete, the baker</t>
-  </si>
-  <si>
-    <t>Extract the domain name from a URL</t>
-  </si>
-  <si>
-    <t>Calculating with Functions</t>
-  </si>
-  <si>
-    <t>The Hashtag Generator</t>
-  </si>
-  <si>
-    <t>Rot13</t>
-  </si>
-  <si>
-    <t>RGB To Hex Conversion</t>
-  </si>
-  <si>
-    <t>Valid Parentheses</t>
-  </si>
-  <si>
-    <t>Moving Zeros To The End</t>
-  </si>
-  <si>
-    <t>Simple Pig Latin</t>
-  </si>
-  <si>
-    <t>N-th Fibonacci</t>
-  </si>
-  <si>
-    <t>Counting Duplicates</t>
-  </si>
-  <si>
-    <t>Bit Counting</t>
-  </si>
-  <si>
-    <t>Stop gninnipS My sdroW!</t>
-  </si>
-  <si>
-    <t>Sum of Digits / Digital Root</t>
-  </si>
-  <si>
-    <t>Find the odd int</t>
-  </si>
-  <si>
-    <t>Who likes it?</t>
-  </si>
-  <si>
-    <t>Multiples of 3 or 5</t>
-  </si>
-  <si>
-    <t>Using Window Functions To Get Top N per Group</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple Hierarchical structure</t>
-  </si>
-  <si>
-    <t>Calculating  Running Total</t>
-  </si>
-  <si>
-    <t>Relational division: Find all movies two actors cast in together</t>
-  </si>
-  <si>
-    <t>SELECT prime numbers</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple PIVOTING data WITHOUT CROSSTAB</t>
-  </si>
-  <si>
-    <t>SQL: Regex AlphaNumeric Split</t>
-  </si>
-  <si>
-    <t>SQL Basics: Create a FUNCTION (DATES)</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple FULL TEXT SEARCH</t>
-  </si>
-  <si>
-    <t>Conditional Count</t>
-  </si>
-  <si>
-    <t>SQL Bug Fixing: Fix the QUERY - Totaling</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple WITH</t>
-  </si>
-  <si>
-    <t>SQL Basics - Monsters using CASE</t>
-  </si>
-  <si>
-    <t>Analyzing the sales by product and date</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple UNION ALL</t>
-  </si>
-  <si>
-    <t>Present XML data the SQL way</t>
-  </si>
-  <si>
-    <t>Calculating Batting Average</t>
-  </si>
-  <si>
-    <t>SQL Basics: Top 10 customers by total payments amount</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple JOIN and RANK</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple EXISTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL Basics: Simple HAVING </t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple NULL handling</t>
-  </si>
-  <si>
-    <t>Challenge: Two actors who cast together the most</t>
-  </si>
-  <si>
-    <t>Countries Capitals for Trivia Night (SQL for Beginners #6)</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple PIVOTING data</t>
-  </si>
-  <si>
-    <t>Present JSON data the SQL way</t>
-  </si>
-  <si>
-    <t>Count Weekdays</t>
-  </si>
-  <si>
-    <t>SQL Statistics: MIN, MEDIAN, MAX</t>
-  </si>
-  <si>
-    <t>SQL Basics: Group By Day</t>
-  </si>
-  <si>
-    <t>Count IP Addresses</t>
-  </si>
-  <si>
-    <t>Subqueries master</t>
-  </si>
-  <si>
-    <t>Using LATERAL JOIN To Get Top N per Group</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple VIEW</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple table totaling.</t>
-  </si>
-  <si>
-    <t>GROCERY STORE: Support Local Products</t>
-  </si>
-  <si>
-    <t>SQL Basics - Trimming the Field</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple IN</t>
-  </si>
-  <si>
-    <t>Nesting Structure Comparison</t>
-  </si>
-  <si>
-    <t>SQL Bug Fixing: Fix the JOIN</t>
-  </si>
-  <si>
-    <t>SQL Basics: Simple JOIN with COUNT</t>
-  </si>
-  <si>
-    <t>Strings Mix</t>
-  </si>
-  <si>
-    <t>Perimeter of squares in a rectangle</t>
-  </si>
-  <si>
-    <t>Directions Reduction</t>
-  </si>
-  <si>
-    <t>Count characters in your string</t>
-  </si>
-  <si>
-    <t>String incrementer</t>
-  </si>
-  <si>
-    <t>Human readable duration format</t>
-  </si>
-  <si>
-    <t>Human Readable Time</t>
-  </si>
-  <si>
-    <t>Where my anagrams at?</t>
-  </si>
-  <si>
-    <t>Strip Comments</t>
-  </si>
-  <si>
-    <t>Write Number in Expanded Form</t>
-  </si>
-  <si>
-    <t>Does my number look big in this?</t>
-  </si>
-  <si>
-    <t>Array.diff</t>
-  </si>
-  <si>
-    <t>Roman Numerals Encoder</t>
-  </si>
-  <si>
-    <t>Consecutive strings</t>
-  </si>
-  <si>
-    <t>Which are  in?</t>
-  </si>
-  <si>
-    <t>Maximum  subarray sum</t>
-  </si>
-  <si>
-    <t>Break camelCase</t>
-  </si>
-  <si>
-    <t>Sum of odd numbers</t>
-  </si>
-  <si>
-    <t>Persistent Bugger.</t>
-  </si>
-  <si>
-    <t>Friend or Foe?</t>
-  </si>
-  <si>
-    <t>Playing with digits</t>
-  </si>
-  <si>
-    <t>Create Phone Number</t>
-  </si>
-  <si>
-    <t>Multiply</t>
-  </si>
-  <si>
-    <t>['python']</t>
-  </si>
-  <si>
-    <t>['sql']</t>
-  </si>
-  <si>
-    <t>Nov-22</t>
-  </si>
-  <si>
-    <t>Oct-22</t>
-  </si>
-  <si>
-    <t>Sep-22</t>
-  </si>
-  <si>
-    <t>Jun-22</t>
-  </si>
-  <si>
-    <t>algorithms</t>
-  </si>
-  <si>
-    <t>games</t>
-  </si>
-  <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>refactoring</t>
-  </si>
-  <si>
-    <t>bug_fixes</t>
-  </si>
-  <si>
-    <t>['Strings', 'Big Integers', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Arrays', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Mathematics', 'Algorithms', 'Puzzles']</t>
-  </si>
-  <si>
-    <t>['Algorithms']</t>
-  </si>
-  <si>
-    <t>['Strings', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Algorithms', 'Mathematics']</t>
-  </si>
-  <si>
-    <t>['Parsing', 'Regular Expressions']</t>
-  </si>
-  <si>
-    <t>['Functional Programming']</t>
-  </si>
-  <si>
-    <t>['Ciphers', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Arrays', 'Sorting', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Regular Expressions', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Strings', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Bits', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Mathematics', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Fundamentals']</t>
-  </si>
-  <si>
-    <t>['SQL', 'Fundamentals', 'Databases']</t>
-  </si>
-  <si>
-    <t>['SQL', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'Databases', 'SQL']</t>
-  </si>
-  <si>
-    <t>['Mathematics', 'Databases']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'SQL', 'Databases']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'Regular Expressions', 'SQL']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'SQL', 'Data Science']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'SQL']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'SQL', 'Databases', 'Data Science']</t>
-  </si>
-  <si>
-    <t>['SQL', 'Data Science', 'JSON']</t>
-  </si>
-  <si>
-    <t>['SQL', 'Statistics', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['SQL', 'Databases', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'Strings']</t>
-  </si>
-  <si>
-    <t>['Regular Expressions', 'Strings']</t>
-  </si>
-  <si>
-    <t>['Strings', 'Date Time', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Date Time', 'Mathematics', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Strings', 'Mathematics', 'Algorithms', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Arrays', 'Fundamentals', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Arrays', 'Lists', 'Strings', 'Refactoring']</t>
-  </si>
-  <si>
-    <t>['Algorithms', 'Lists', 'Dynamic Programming', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Arrays', 'Lists', 'Mathematics', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>['Fundamentals', 'Mathematics']</t>
-  </si>
-  <si>
-    <t>['Arrays', 'Strings', 'Regular Expressions', 'Algorithms']</t>
-  </si>
-  <si>
-    <t>['Debugging', 'Fundamentals']</t>
-  </si>
-  <si>
-    <t>5 kyu</t>
-  </si>
-  <si>
-    <t>6 kyu</t>
-  </si>
-  <si>
-    <t>7 kyu</t>
-  </si>
-  <si>
-    <t>8 kyu</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>Kata Compeleted By Filpill since 12-Nov-2022</t>
-  </si>
-  <si>
-    <t>Kata ID</t>
-  </si>
-  <si>
-    <t>Kata Name</t>
-  </si>
-  <si>
-    <t>Languages</t>
-  </si>
-  <si>
-    <t>Completed Date</t>
-  </si>
-  <si>
-    <t>Completion Period</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Total Attempts</t>
   </si>
   <si>
     <t>Tags</t>
@@ -894,7 +897,7 @@
     <tableColumn id="5" name="Total Score"/>
     <tableColumn id="6" name="Python Score"/>
     <tableColumn id="7" name="SQL Score"/>
-    <tableColumn id="8" name="Total Completed"/>
+    <tableColumn id="8" name="codeChallenges.totalCompleted"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1270,7 +1273,7 @@
         <v>1016</v>
       </c>
       <c r="D4">
-        <v>23238</v>
+        <v>23246</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1326,16 +1329,16 @@
         <v>247</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>10</v>
+        <v>248</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -1358,10 +1361,10 @@
         <v>189</v>
       </c>
       <c r="H10">
-        <v>490630</v>
+        <v>490952</v>
       </c>
       <c r="I10">
-        <v>28848</v>
+        <v>28871</v>
       </c>
       <c r="J10" t="s">
         <v>194</v>
@@ -1393,10 +1396,10 @@
         <v>189</v>
       </c>
       <c r="H11">
-        <v>401079</v>
+        <v>401296</v>
       </c>
       <c r="I11">
-        <v>53787</v>
+        <v>53804</v>
       </c>
       <c r="J11" t="s">
         <v>195</v>
@@ -1428,10 +1431,10 @@
         <v>190</v>
       </c>
       <c r="H12">
-        <v>84565</v>
+        <v>84579</v>
       </c>
       <c r="I12">
-        <v>5877</v>
+        <v>5878</v>
       </c>
       <c r="J12" t="s">
         <v>196</v>
@@ -1463,10 +1466,10 @@
         <v>189</v>
       </c>
       <c r="H13">
-        <v>310962</v>
+        <v>310984</v>
       </c>
       <c r="I13">
-        <v>41314</v>
+        <v>41320</v>
       </c>
       <c r="J13" t="s">
         <v>197</v>
@@ -1498,10 +1501,10 @@
         <v>189</v>
       </c>
       <c r="H14">
-        <v>288208</v>
+        <v>288336</v>
       </c>
       <c r="I14">
-        <v>45616</v>
+        <v>45636</v>
       </c>
       <c r="J14" t="s">
         <v>198</v>
@@ -1533,10 +1536,10 @@
         <v>191</v>
       </c>
       <c r="H15">
-        <v>182903</v>
+        <v>182951</v>
       </c>
       <c r="I15">
-        <v>49233</v>
+        <v>49244</v>
       </c>
       <c r="J15" t="s">
         <v>199</v>
@@ -1568,10 +1571,10 @@
         <v>189</v>
       </c>
       <c r="H16">
-        <v>182245</v>
+        <v>182323</v>
       </c>
       <c r="I16">
-        <v>50110</v>
+        <v>50129</v>
       </c>
       <c r="J16" t="s">
         <v>197</v>
@@ -1603,10 +1606,10 @@
         <v>191</v>
       </c>
       <c r="H17">
-        <v>383176</v>
+        <v>383510</v>
       </c>
       <c r="I17">
-        <v>52001</v>
+        <v>52042</v>
       </c>
       <c r="J17" t="s">
         <v>200</v>
@@ -1638,10 +1641,10 @@
         <v>191</v>
       </c>
       <c r="H18">
-        <v>223071</v>
+        <v>223173</v>
       </c>
       <c r="I18">
-        <v>58571</v>
+        <v>58590</v>
       </c>
       <c r="J18" t="s">
         <v>201</v>
@@ -1673,10 +1676,10 @@
         <v>189</v>
       </c>
       <c r="H19">
-        <v>228563</v>
+        <v>228681</v>
       </c>
       <c r="I19">
-        <v>59443</v>
+        <v>59478</v>
       </c>
       <c r="J19" t="s">
         <v>198</v>
@@ -1708,10 +1711,10 @@
         <v>191</v>
       </c>
       <c r="H20">
-        <v>322215</v>
+        <v>322294</v>
       </c>
       <c r="I20">
-        <v>64665</v>
+        <v>64683</v>
       </c>
       <c r="J20" t="s">
         <v>202</v>
@@ -1743,10 +1746,10 @@
         <v>189</v>
       </c>
       <c r="H21">
-        <v>338036</v>
+        <v>338108</v>
       </c>
       <c r="I21">
-        <v>87574</v>
+        <v>87600</v>
       </c>
       <c r="J21" t="s">
         <v>197</v>
@@ -1778,10 +1781,10 @@
         <v>189</v>
       </c>
       <c r="H22">
-        <v>534830</v>
+        <v>534993</v>
       </c>
       <c r="I22">
-        <v>88948</v>
+        <v>88980</v>
       </c>
       <c r="J22" t="s">
         <v>197</v>
@@ -1813,10 +1816,10 @@
         <v>189</v>
       </c>
       <c r="H23">
-        <v>479195</v>
+        <v>479352</v>
       </c>
       <c r="I23">
-        <v>114357</v>
+        <v>114415</v>
       </c>
       <c r="J23" t="s">
         <v>203</v>
@@ -1848,10 +1851,10 @@
         <v>189</v>
       </c>
       <c r="H24">
-        <v>634296</v>
+        <v>634541</v>
       </c>
       <c r="I24">
-        <v>115539</v>
+        <v>115582</v>
       </c>
       <c r="J24" t="s">
         <v>204</v>
@@ -1883,10 +1886,10 @@
         <v>189</v>
       </c>
       <c r="H25">
-        <v>48828</v>
+        <v>48852</v>
       </c>
       <c r="I25">
-        <v>14520</v>
+        <v>14532</v>
       </c>
       <c r="J25" t="s">
         <v>197</v>
@@ -1918,10 +1921,10 @@
         <v>191</v>
       </c>
       <c r="H26">
-        <v>677375</v>
+        <v>677513</v>
       </c>
       <c r="I26">
-        <v>163292</v>
+        <v>163337</v>
       </c>
       <c r="J26" t="s">
         <v>205</v>
@@ -1953,10 +1956,10 @@
         <v>189</v>
       </c>
       <c r="H27">
-        <v>431629</v>
+        <v>431749</v>
       </c>
       <c r="I27">
-        <v>175437</v>
+        <v>175487</v>
       </c>
       <c r="J27" t="s">
         <v>206</v>
@@ -1988,10 +1991,10 @@
         <v>189</v>
       </c>
       <c r="H28">
-        <v>701405</v>
+        <v>701670</v>
       </c>
       <c r="I28">
-        <v>191483</v>
+        <v>191546</v>
       </c>
       <c r="J28" t="s">
         <v>198</v>
@@ -2023,10 +2026,10 @@
         <v>189</v>
       </c>
       <c r="H29">
-        <v>785080</v>
+        <v>785317</v>
       </c>
       <c r="I29">
-        <v>197177</v>
+        <v>197234</v>
       </c>
       <c r="J29" t="s">
         <v>207</v>
@@ -2058,10 +2061,10 @@
         <v>191</v>
       </c>
       <c r="H30">
-        <v>634629</v>
+        <v>634698</v>
       </c>
       <c r="I30">
-        <v>215114</v>
+        <v>215163</v>
       </c>
       <c r="J30" t="s">
         <v>208</v>
@@ -2093,10 +2096,10 @@
         <v>191</v>
       </c>
       <c r="H31">
-        <v>724739</v>
+        <v>724924</v>
       </c>
       <c r="I31">
-        <v>233289</v>
+        <v>233374</v>
       </c>
       <c r="J31" t="s">
         <v>205</v>
@@ -2128,10 +2131,10 @@
         <v>189</v>
       </c>
       <c r="H32">
-        <v>884253</v>
+        <v>884476</v>
       </c>
       <c r="I32">
-        <v>295556</v>
+        <v>295661</v>
       </c>
       <c r="J32" t="s">
         <v>207</v>
@@ -2233,10 +2236,10 @@
         <v>191</v>
       </c>
       <c r="H35">
-        <v>27816</v>
+        <v>27818</v>
       </c>
       <c r="I35">
-        <v>3621</v>
+        <v>3623</v>
       </c>
       <c r="J35" t="s">
         <v>211</v>
@@ -2268,10 +2271,10 @@
         <v>191</v>
       </c>
       <c r="H36">
-        <v>27200</v>
+        <v>27201</v>
       </c>
       <c r="I36">
-        <v>6028</v>
+        <v>6029</v>
       </c>
       <c r="J36" t="s">
         <v>211</v>
@@ -2408,10 +2411,10 @@
         <v>191</v>
       </c>
       <c r="H40">
-        <v>44081</v>
+        <v>44099</v>
       </c>
       <c r="I40">
-        <v>2877</v>
+        <v>2878</v>
       </c>
       <c r="J40" t="s">
         <v>210</v>
@@ -2478,10 +2481,10 @@
         <v>191</v>
       </c>
       <c r="H42">
-        <v>36517</v>
+        <v>36518</v>
       </c>
       <c r="I42">
-        <v>5809</v>
+        <v>5810</v>
       </c>
       <c r="J42" t="s">
         <v>209</v>
@@ -2618,7 +2621,7 @@
         <v>189</v>
       </c>
       <c r="H46">
-        <v>17867</v>
+        <v>17878</v>
       </c>
       <c r="I46">
         <v>1765</v>
@@ -2653,10 +2656,10 @@
         <v>191</v>
       </c>
       <c r="H47">
-        <v>51247</v>
+        <v>51262</v>
       </c>
       <c r="I47">
-        <v>9949</v>
+        <v>9952</v>
       </c>
       <c r="J47" t="s">
         <v>210</v>
@@ -2688,10 +2691,10 @@
         <v>191</v>
       </c>
       <c r="H48">
-        <v>3572</v>
+        <v>3574</v>
       </c>
       <c r="I48">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="J48" t="s">
         <v>215</v>
@@ -2723,10 +2726,10 @@
         <v>191</v>
       </c>
       <c r="H49">
-        <v>42050</v>
+        <v>42051</v>
       </c>
       <c r="I49">
-        <v>4642</v>
+        <v>4643</v>
       </c>
       <c r="J49" t="s">
         <v>210</v>
@@ -2758,10 +2761,10 @@
         <v>191</v>
       </c>
       <c r="H50">
-        <v>43200</v>
+        <v>43249</v>
       </c>
       <c r="I50">
-        <v>10496</v>
+        <v>10501</v>
       </c>
       <c r="J50" t="s">
         <v>215</v>
@@ -2793,10 +2796,10 @@
         <v>191</v>
       </c>
       <c r="H51">
-        <v>56104</v>
+        <v>56107</v>
       </c>
       <c r="I51">
-        <v>10536</v>
+        <v>10538</v>
       </c>
       <c r="J51" t="s">
         <v>210</v>
@@ -2828,10 +2831,10 @@
         <v>191</v>
       </c>
       <c r="H52">
-        <v>62363</v>
+        <v>62368</v>
       </c>
       <c r="I52">
-        <v>10774</v>
+        <v>10775</v>
       </c>
       <c r="J52" t="s">
         <v>210</v>
@@ -2863,10 +2866,10 @@
         <v>191</v>
       </c>
       <c r="H53">
-        <v>37001</v>
+        <v>37004</v>
       </c>
       <c r="I53">
-        <v>15085</v>
+        <v>15087</v>
       </c>
       <c r="J53" t="s">
         <v>210</v>
@@ -2898,10 +2901,10 @@
         <v>191</v>
       </c>
       <c r="H54">
-        <v>40808</v>
+        <v>40825</v>
       </c>
       <c r="I54">
-        <v>6523</v>
+        <v>6525</v>
       </c>
       <c r="J54" t="s">
         <v>210</v>
@@ -2933,10 +2936,10 @@
         <v>191</v>
       </c>
       <c r="H55">
-        <v>30866</v>
+        <v>30888</v>
       </c>
       <c r="I55">
-        <v>2631</v>
+        <v>2632</v>
       </c>
       <c r="J55" t="s">
         <v>209</v>
@@ -2968,10 +2971,10 @@
         <v>191</v>
       </c>
       <c r="H56">
-        <v>37021</v>
+        <v>37026</v>
       </c>
       <c r="I56">
-        <v>8319</v>
+        <v>8322</v>
       </c>
       <c r="J56" t="s">
         <v>217</v>
@@ -3038,10 +3041,10 @@
         <v>191</v>
       </c>
       <c r="H58">
-        <v>9334</v>
+        <v>9390</v>
       </c>
       <c r="I58">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="J58" t="s">
         <v>218</v>
@@ -3073,7 +3076,7 @@
         <v>191</v>
       </c>
       <c r="H59">
-        <v>26976</v>
+        <v>26977</v>
       </c>
       <c r="I59">
         <v>1151</v>
@@ -3108,10 +3111,10 @@
         <v>191</v>
       </c>
       <c r="H60">
-        <v>32522</v>
+        <v>32524</v>
       </c>
       <c r="I60">
-        <v>4731</v>
+        <v>4732</v>
       </c>
       <c r="J60" t="s">
         <v>219</v>
@@ -3143,10 +3146,10 @@
         <v>191</v>
       </c>
       <c r="H61">
-        <v>29128</v>
+        <v>29129</v>
       </c>
       <c r="I61">
-        <v>6052</v>
+        <v>6053</v>
       </c>
       <c r="J61" t="s">
         <v>210</v>
@@ -3178,10 +3181,10 @@
         <v>189</v>
       </c>
       <c r="H62">
-        <v>62774</v>
+        <v>62816</v>
       </c>
       <c r="I62">
-        <v>16433</v>
+        <v>16439</v>
       </c>
       <c r="J62" t="s">
         <v>197</v>
@@ -3283,10 +3286,10 @@
         <v>191</v>
       </c>
       <c r="H65">
-        <v>34360</v>
+        <v>34363</v>
       </c>
       <c r="I65">
-        <v>3274</v>
+        <v>3276</v>
       </c>
       <c r="J65" t="s">
         <v>210</v>
@@ -3318,10 +3321,10 @@
         <v>191</v>
       </c>
       <c r="H66">
-        <v>73805</v>
+        <v>73810</v>
       </c>
       <c r="I66">
-        <v>8200</v>
+        <v>8201</v>
       </c>
       <c r="J66" t="s">
         <v>210</v>
@@ -3388,10 +3391,10 @@
         <v>191</v>
       </c>
       <c r="H68">
-        <v>35068</v>
+        <v>35073</v>
       </c>
       <c r="I68">
-        <v>5881</v>
+        <v>5883</v>
       </c>
       <c r="J68" t="s">
         <v>216</v>
@@ -3423,10 +3426,10 @@
         <v>191</v>
       </c>
       <c r="H69">
-        <v>52024</v>
+        <v>52025</v>
       </c>
       <c r="I69">
-        <v>10470</v>
+        <v>10471</v>
       </c>
       <c r="J69" t="s">
         <v>210</v>
@@ -3458,10 +3461,10 @@
         <v>189</v>
       </c>
       <c r="H70">
-        <v>183331</v>
+        <v>183405</v>
       </c>
       <c r="I70">
-        <v>15338</v>
+        <v>15344</v>
       </c>
       <c r="J70" t="s">
         <v>195</v>
@@ -3528,10 +3531,10 @@
         <v>191</v>
       </c>
       <c r="H72">
-        <v>58942</v>
+        <v>58947</v>
       </c>
       <c r="I72">
-        <v>15408</v>
+        <v>15413</v>
       </c>
       <c r="J72" t="s">
         <v>220</v>
@@ -3563,10 +3566,10 @@
         <v>191</v>
       </c>
       <c r="H73">
-        <v>144235</v>
+        <v>144254</v>
       </c>
       <c r="I73">
-        <v>18316</v>
+        <v>18319</v>
       </c>
       <c r="J73" t="s">
         <v>221</v>
@@ -3598,10 +3601,10 @@
         <v>189</v>
       </c>
       <c r="H74">
-        <v>108918</v>
+        <v>108947</v>
       </c>
       <c r="I74">
-        <v>30868</v>
+        <v>30873</v>
       </c>
       <c r="J74" t="s">
         <v>207</v>
@@ -3633,10 +3636,10 @@
         <v>191</v>
       </c>
       <c r="H75">
-        <v>450877</v>
+        <v>451018</v>
       </c>
       <c r="I75">
-        <v>65992</v>
+        <v>66011</v>
       </c>
       <c r="J75" t="s">
         <v>208</v>
@@ -3668,10 +3671,10 @@
         <v>191</v>
       </c>
       <c r="H76">
-        <v>121312</v>
+        <v>121325</v>
       </c>
       <c r="I76">
-        <v>53047</v>
+        <v>53056</v>
       </c>
       <c r="J76" t="s">
         <v>205</v>
@@ -3703,10 +3706,10 @@
         <v>191</v>
       </c>
       <c r="H77">
-        <v>322427</v>
+        <v>322492</v>
       </c>
       <c r="I77">
-        <v>32335</v>
+        <v>32343</v>
       </c>
       <c r="J77" t="s">
         <v>222</v>
@@ -3738,10 +3741,10 @@
         <v>189</v>
       </c>
       <c r="H78">
-        <v>461758</v>
+        <v>461929</v>
       </c>
       <c r="I78">
-        <v>57480</v>
+        <v>57516</v>
       </c>
       <c r="J78" t="s">
         <v>223</v>
@@ -3773,10 +3776,10 @@
         <v>189</v>
       </c>
       <c r="H79">
-        <v>276659</v>
+        <v>276711</v>
       </c>
       <c r="I79">
-        <v>99137</v>
+        <v>99165</v>
       </c>
       <c r="J79" t="s">
         <v>224</v>
@@ -3843,10 +3846,10 @@
         <v>189</v>
       </c>
       <c r="H81">
-        <v>380213</v>
+        <v>380283</v>
       </c>
       <c r="I81">
-        <v>38652</v>
+        <v>38661</v>
       </c>
       <c r="J81" t="s">
         <v>198</v>
@@ -3878,10 +3881,10 @@
         <v>191</v>
       </c>
       <c r="H82">
-        <v>235807</v>
+        <v>235867</v>
       </c>
       <c r="I82">
-        <v>54306</v>
+        <v>54323</v>
       </c>
       <c r="J82" t="s">
         <v>225</v>
@@ -3913,10 +3916,10 @@
         <v>189</v>
       </c>
       <c r="H83">
-        <v>312092</v>
+        <v>312191</v>
       </c>
       <c r="I83">
-        <v>110368</v>
+        <v>110410</v>
       </c>
       <c r="J83" t="s">
         <v>197</v>
@@ -3948,10 +3951,10 @@
         <v>191</v>
       </c>
       <c r="H84">
-        <v>711839</v>
+        <v>712107</v>
       </c>
       <c r="I84">
-        <v>191802</v>
+        <v>191859</v>
       </c>
       <c r="J84" t="s">
         <v>226</v>
@@ -3983,10 +3986,10 @@
         <v>189</v>
       </c>
       <c r="H85">
-        <v>170133</v>
+        <v>170158</v>
       </c>
       <c r="I85">
-        <v>39815</v>
+        <v>39823</v>
       </c>
       <c r="J85" t="s">
         <v>197</v>
@@ -4018,10 +4021,10 @@
         <v>191</v>
       </c>
       <c r="H86">
-        <v>428274</v>
+        <v>428365</v>
       </c>
       <c r="I86">
-        <v>59019</v>
+        <v>59038</v>
       </c>
       <c r="J86" t="s">
         <v>208</v>
@@ -4053,10 +4056,10 @@
         <v>192</v>
       </c>
       <c r="H87">
-        <v>289086</v>
+        <v>289120</v>
       </c>
       <c r="I87">
-        <v>62031</v>
+        <v>62044</v>
       </c>
       <c r="J87" t="s">
         <v>227</v>
@@ -4088,10 +4091,10 @@
         <v>191</v>
       </c>
       <c r="H88">
-        <v>324904</v>
+        <v>324943</v>
       </c>
       <c r="I88">
-        <v>58355</v>
+        <v>58366</v>
       </c>
       <c r="J88" t="s">
         <v>228</v>
@@ -4123,10 +4126,10 @@
         <v>191</v>
       </c>
       <c r="H89">
-        <v>184009</v>
+        <v>184118</v>
       </c>
       <c r="I89">
-        <v>67578</v>
+        <v>67621</v>
       </c>
       <c r="J89" t="s">
         <v>205</v>
@@ -4158,10 +4161,10 @@
         <v>191</v>
       </c>
       <c r="H90">
-        <v>313611</v>
+        <v>313671</v>
       </c>
       <c r="I90">
-        <v>115620</v>
+        <v>115655</v>
       </c>
       <c r="J90" t="s">
         <v>229</v>
@@ -4193,10 +4196,10 @@
         <v>191</v>
       </c>
       <c r="H91">
-        <v>503124</v>
+        <v>503209</v>
       </c>
       <c r="I91">
-        <v>141035</v>
+        <v>141069</v>
       </c>
       <c r="J91" t="s">
         <v>208</v>
@@ -4228,10 +4231,10 @@
         <v>191</v>
       </c>
       <c r="H92">
-        <v>278730</v>
+        <v>278826</v>
       </c>
       <c r="I92">
-        <v>124744</v>
+        <v>124793</v>
       </c>
       <c r="J92" t="s">
         <v>208</v>
@@ -4263,10 +4266,10 @@
         <v>191</v>
       </c>
       <c r="H93">
-        <v>395372</v>
+        <v>395439</v>
       </c>
       <c r="I93">
-        <v>102344</v>
+        <v>102364</v>
       </c>
       <c r="J93" t="s">
         <v>230</v>
@@ -4298,10 +4301,10 @@
         <v>189</v>
       </c>
       <c r="H94">
-        <v>556882</v>
+        <v>557091</v>
       </c>
       <c r="I94">
-        <v>230289</v>
+        <v>230361</v>
       </c>
       <c r="J94" t="s">
         <v>231</v>
@@ -4333,10 +4336,10 @@
         <v>193</v>
       </c>
       <c r="H95">
-        <v>6447234</v>
+        <v>6447739</v>
       </c>
       <c r="I95">
-        <v>5327439</v>
+        <v>5327832</v>
       </c>
       <c r="J95" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
created all subsets of visualisations
</commit_message>
<xml_diff>
--- a/xlsx_data/codewars_stats_Filpill.xlsx
+++ b/xlsx_data/codewars_stats_Filpill.xlsx
@@ -1273,7 +1273,7 @@
         <v>1016</v>
       </c>
       <c r="D4">
-        <v>23246</v>
+        <v>23252</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1361,10 +1361,10 @@
         <v>189</v>
       </c>
       <c r="H10">
-        <v>490952</v>
+        <v>491483</v>
       </c>
       <c r="I10">
-        <v>28871</v>
+        <v>28893</v>
       </c>
       <c r="J10" t="s">
         <v>194</v>
@@ -1396,10 +1396,10 @@
         <v>189</v>
       </c>
       <c r="H11">
-        <v>401296</v>
+        <v>401376</v>
       </c>
       <c r="I11">
-        <v>53804</v>
+        <v>53820</v>
       </c>
       <c r="J11" t="s">
         <v>195</v>
@@ -1431,10 +1431,10 @@
         <v>190</v>
       </c>
       <c r="H12">
-        <v>84579</v>
+        <v>84617</v>
       </c>
       <c r="I12">
-        <v>5878</v>
+        <v>5879</v>
       </c>
       <c r="J12" t="s">
         <v>196</v>
@@ -1466,10 +1466,10 @@
         <v>189</v>
       </c>
       <c r="H13">
-        <v>310984</v>
+        <v>311040</v>
       </c>
       <c r="I13">
-        <v>41320</v>
+        <v>41325</v>
       </c>
       <c r="J13" t="s">
         <v>197</v>
@@ -1501,10 +1501,10 @@
         <v>189</v>
       </c>
       <c r="H14">
-        <v>288336</v>
+        <v>288383</v>
       </c>
       <c r="I14">
-        <v>45636</v>
+        <v>45649</v>
       </c>
       <c r="J14" t="s">
         <v>198</v>
@@ -1536,10 +1536,10 @@
         <v>191</v>
       </c>
       <c r="H15">
-        <v>182951</v>
+        <v>182978</v>
       </c>
       <c r="I15">
-        <v>49244</v>
+        <v>49256</v>
       </c>
       <c r="J15" t="s">
         <v>199</v>
@@ -1571,10 +1571,10 @@
         <v>189</v>
       </c>
       <c r="H16">
-        <v>182323</v>
+        <v>182453</v>
       </c>
       <c r="I16">
-        <v>50129</v>
+        <v>50149</v>
       </c>
       <c r="J16" t="s">
         <v>197</v>
@@ -1606,10 +1606,10 @@
         <v>191</v>
       </c>
       <c r="H17">
-        <v>383510</v>
+        <v>383594</v>
       </c>
       <c r="I17">
-        <v>52042</v>
+        <v>52058</v>
       </c>
       <c r="J17" t="s">
         <v>200</v>
@@ -1641,10 +1641,10 @@
         <v>191</v>
       </c>
       <c r="H18">
-        <v>223173</v>
+        <v>223230</v>
       </c>
       <c r="I18">
-        <v>58590</v>
+        <v>58611</v>
       </c>
       <c r="J18" t="s">
         <v>201</v>
@@ -1676,10 +1676,10 @@
         <v>189</v>
       </c>
       <c r="H19">
-        <v>228681</v>
+        <v>228744</v>
       </c>
       <c r="I19">
-        <v>59478</v>
+        <v>59500</v>
       </c>
       <c r="J19" t="s">
         <v>198</v>
@@ -1711,10 +1711,10 @@
         <v>191</v>
       </c>
       <c r="H20">
-        <v>322294</v>
+        <v>322422</v>
       </c>
       <c r="I20">
-        <v>64683</v>
+        <v>64703</v>
       </c>
       <c r="J20" t="s">
         <v>202</v>
@@ -1746,10 +1746,10 @@
         <v>189</v>
       </c>
       <c r="H21">
-        <v>338108</v>
+        <v>338294</v>
       </c>
       <c r="I21">
-        <v>87600</v>
+        <v>87634</v>
       </c>
       <c r="J21" t="s">
         <v>197</v>
@@ -1781,10 +1781,10 @@
         <v>189</v>
       </c>
       <c r="H22">
-        <v>534993</v>
+        <v>535311</v>
       </c>
       <c r="I22">
-        <v>88980</v>
+        <v>89011</v>
       </c>
       <c r="J22" t="s">
         <v>197</v>
@@ -1816,10 +1816,10 @@
         <v>189</v>
       </c>
       <c r="H23">
-        <v>479352</v>
+        <v>479548</v>
       </c>
       <c r="I23">
-        <v>114415</v>
+        <v>114460</v>
       </c>
       <c r="J23" t="s">
         <v>203</v>
@@ -1851,10 +1851,10 @@
         <v>189</v>
       </c>
       <c r="H24">
-        <v>634541</v>
+        <v>634760</v>
       </c>
       <c r="I24">
-        <v>115582</v>
+        <v>115618</v>
       </c>
       <c r="J24" t="s">
         <v>204</v>
@@ -1886,10 +1886,10 @@
         <v>189</v>
       </c>
       <c r="H25">
-        <v>48852</v>
+        <v>48864</v>
       </c>
       <c r="I25">
-        <v>14532</v>
+        <v>14541</v>
       </c>
       <c r="J25" t="s">
         <v>197</v>
@@ -1921,10 +1921,10 @@
         <v>191</v>
       </c>
       <c r="H26">
-        <v>677513</v>
+        <v>677698</v>
       </c>
       <c r="I26">
-        <v>163337</v>
+        <v>163394</v>
       </c>
       <c r="J26" t="s">
         <v>205</v>
@@ -1956,10 +1956,10 @@
         <v>189</v>
       </c>
       <c r="H27">
-        <v>431749</v>
+        <v>431847</v>
       </c>
       <c r="I27">
-        <v>175487</v>
+        <v>175531</v>
       </c>
       <c r="J27" t="s">
         <v>206</v>
@@ -1991,10 +1991,10 @@
         <v>189</v>
       </c>
       <c r="H28">
-        <v>701670</v>
+        <v>701813</v>
       </c>
       <c r="I28">
-        <v>191546</v>
+        <v>191605</v>
       </c>
       <c r="J28" t="s">
         <v>198</v>
@@ -2026,10 +2026,10 @@
         <v>189</v>
       </c>
       <c r="H29">
-        <v>785317</v>
+        <v>785539</v>
       </c>
       <c r="I29">
-        <v>197234</v>
+        <v>197300</v>
       </c>
       <c r="J29" t="s">
         <v>207</v>
@@ -2061,10 +2061,10 @@
         <v>191</v>
       </c>
       <c r="H30">
-        <v>634698</v>
+        <v>634824</v>
       </c>
       <c r="I30">
-        <v>215163</v>
+        <v>215229</v>
       </c>
       <c r="J30" t="s">
         <v>208</v>
@@ -2096,10 +2096,10 @@
         <v>191</v>
       </c>
       <c r="H31">
-        <v>724924</v>
+        <v>725075</v>
       </c>
       <c r="I31">
-        <v>233374</v>
+        <v>233456</v>
       </c>
       <c r="J31" t="s">
         <v>205</v>
@@ -2131,10 +2131,10 @@
         <v>189</v>
       </c>
       <c r="H32">
-        <v>884476</v>
+        <v>884752</v>
       </c>
       <c r="I32">
-        <v>295661</v>
+        <v>295780</v>
       </c>
       <c r="J32" t="s">
         <v>207</v>
@@ -2166,10 +2166,10 @@
         <v>191</v>
       </c>
       <c r="H33">
-        <v>22823</v>
+        <v>22825</v>
       </c>
       <c r="I33">
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="J33" t="s">
         <v>209</v>
@@ -2271,10 +2271,10 @@
         <v>191</v>
       </c>
       <c r="H36">
-        <v>27201</v>
+        <v>27205</v>
       </c>
       <c r="I36">
-        <v>6029</v>
+        <v>6033</v>
       </c>
       <c r="J36" t="s">
         <v>211</v>
@@ -2306,7 +2306,7 @@
         <v>190</v>
       </c>
       <c r="H37">
-        <v>29821</v>
+        <v>29822</v>
       </c>
       <c r="I37">
         <v>2202</v>
@@ -2341,10 +2341,10 @@
         <v>191</v>
       </c>
       <c r="H38">
-        <v>13036</v>
+        <v>13037</v>
       </c>
       <c r="I38">
-        <v>2665</v>
+        <v>2666</v>
       </c>
       <c r="J38" t="s">
         <v>213</v>
@@ -2376,10 +2376,10 @@
         <v>191</v>
       </c>
       <c r="H39">
-        <v>19491</v>
+        <v>19493</v>
       </c>
       <c r="I39">
-        <v>2680</v>
+        <v>2681</v>
       </c>
       <c r="J39" t="s">
         <v>214</v>
@@ -2446,10 +2446,10 @@
         <v>191</v>
       </c>
       <c r="H41">
-        <v>10865</v>
+        <v>10867</v>
       </c>
       <c r="I41">
-        <v>3804</v>
+        <v>3806</v>
       </c>
       <c r="J41" t="s">
         <v>210</v>
@@ -2481,10 +2481,10 @@
         <v>191</v>
       </c>
       <c r="H42">
-        <v>36518</v>
+        <v>36519</v>
       </c>
       <c r="I42">
-        <v>5810</v>
+        <v>5811</v>
       </c>
       <c r="J42" t="s">
         <v>209</v>
@@ -2516,10 +2516,10 @@
         <v>191</v>
       </c>
       <c r="H43">
-        <v>32102</v>
+        <v>32105</v>
       </c>
       <c r="I43">
-        <v>7066</v>
+        <v>7068</v>
       </c>
       <c r="J43" t="s">
         <v>215</v>
@@ -2551,10 +2551,10 @@
         <v>191</v>
       </c>
       <c r="H44">
-        <v>27258</v>
+        <v>27259</v>
       </c>
       <c r="I44">
-        <v>7104</v>
+        <v>7105</v>
       </c>
       <c r="J44" t="s">
         <v>210</v>
@@ -2586,10 +2586,10 @@
         <v>191</v>
       </c>
       <c r="H45">
-        <v>35626</v>
+        <v>35637</v>
       </c>
       <c r="I45">
-        <v>8779</v>
+        <v>8782</v>
       </c>
       <c r="J45" t="s">
         <v>216</v>
@@ -2621,10 +2621,10 @@
         <v>189</v>
       </c>
       <c r="H46">
-        <v>17878</v>
+        <v>17881</v>
       </c>
       <c r="I46">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="J46" t="s">
         <v>197</v>
@@ -2656,10 +2656,10 @@
         <v>191</v>
       </c>
       <c r="H47">
-        <v>51262</v>
+        <v>51264</v>
       </c>
       <c r="I47">
-        <v>9952</v>
+        <v>9953</v>
       </c>
       <c r="J47" t="s">
         <v>210</v>
@@ -2726,10 +2726,10 @@
         <v>191</v>
       </c>
       <c r="H49">
-        <v>42051</v>
+        <v>42052</v>
       </c>
       <c r="I49">
-        <v>4643</v>
+        <v>4644</v>
       </c>
       <c r="J49" t="s">
         <v>210</v>
@@ -2761,10 +2761,10 @@
         <v>191</v>
       </c>
       <c r="H50">
-        <v>43249</v>
+        <v>43266</v>
       </c>
       <c r="I50">
-        <v>10501</v>
+        <v>10504</v>
       </c>
       <c r="J50" t="s">
         <v>215</v>
@@ -2796,10 +2796,10 @@
         <v>191</v>
       </c>
       <c r="H51">
-        <v>56107</v>
+        <v>56109</v>
       </c>
       <c r="I51">
-        <v>10538</v>
+        <v>10540</v>
       </c>
       <c r="J51" t="s">
         <v>210</v>
@@ -2831,10 +2831,10 @@
         <v>191</v>
       </c>
       <c r="H52">
-        <v>62368</v>
+        <v>62370</v>
       </c>
       <c r="I52">
-        <v>10775</v>
+        <v>10777</v>
       </c>
       <c r="J52" t="s">
         <v>210</v>
@@ -2901,10 +2901,10 @@
         <v>191</v>
       </c>
       <c r="H54">
-        <v>40825</v>
+        <v>40827</v>
       </c>
       <c r="I54">
-        <v>6525</v>
+        <v>6527</v>
       </c>
       <c r="J54" t="s">
         <v>210</v>
@@ -2936,10 +2936,10 @@
         <v>191</v>
       </c>
       <c r="H55">
-        <v>30888</v>
+        <v>30892</v>
       </c>
       <c r="I55">
-        <v>2632</v>
+        <v>2634</v>
       </c>
       <c r="J55" t="s">
         <v>209</v>
@@ -2971,10 +2971,10 @@
         <v>191</v>
       </c>
       <c r="H56">
-        <v>37026</v>
+        <v>37060</v>
       </c>
       <c r="I56">
-        <v>8322</v>
+        <v>8327</v>
       </c>
       <c r="J56" t="s">
         <v>217</v>
@@ -3076,7 +3076,7 @@
         <v>191</v>
       </c>
       <c r="H59">
-        <v>26977</v>
+        <v>26986</v>
       </c>
       <c r="I59">
         <v>1151</v>
@@ -3111,10 +3111,10 @@
         <v>191</v>
       </c>
       <c r="H60">
-        <v>32524</v>
+        <v>32526</v>
       </c>
       <c r="I60">
-        <v>4732</v>
+        <v>4734</v>
       </c>
       <c r="J60" t="s">
         <v>219</v>
@@ -3181,10 +3181,10 @@
         <v>189</v>
       </c>
       <c r="H62">
-        <v>62816</v>
+        <v>62831</v>
       </c>
       <c r="I62">
-        <v>16439</v>
+        <v>16448</v>
       </c>
       <c r="J62" t="s">
         <v>197</v>
@@ -3286,7 +3286,7 @@
         <v>191</v>
       </c>
       <c r="H65">
-        <v>34363</v>
+        <v>34364</v>
       </c>
       <c r="I65">
         <v>3276</v>
@@ -3356,10 +3356,10 @@
         <v>191</v>
       </c>
       <c r="H67">
-        <v>28298</v>
+        <v>28299</v>
       </c>
       <c r="I67">
-        <v>6627</v>
+        <v>6628</v>
       </c>
       <c r="J67" t="s">
         <v>220</v>
@@ -3391,10 +3391,10 @@
         <v>191</v>
       </c>
       <c r="H68">
-        <v>35073</v>
+        <v>35078</v>
       </c>
       <c r="I68">
-        <v>5883</v>
+        <v>5885</v>
       </c>
       <c r="J68" t="s">
         <v>216</v>
@@ -3461,10 +3461,10 @@
         <v>189</v>
       </c>
       <c r="H70">
-        <v>183405</v>
+        <v>183422</v>
       </c>
       <c r="I70">
-        <v>15344</v>
+        <v>15346</v>
       </c>
       <c r="J70" t="s">
         <v>195</v>
@@ -3496,10 +3496,10 @@
         <v>191</v>
       </c>
       <c r="H71">
-        <v>85460</v>
+        <v>85496</v>
       </c>
       <c r="I71">
-        <v>7492</v>
+        <v>7494</v>
       </c>
       <c r="J71" t="s">
         <v>210</v>
@@ -3531,10 +3531,10 @@
         <v>191</v>
       </c>
       <c r="H72">
-        <v>58947</v>
+        <v>58953</v>
       </c>
       <c r="I72">
-        <v>15413</v>
+        <v>15417</v>
       </c>
       <c r="J72" t="s">
         <v>220</v>
@@ -3566,10 +3566,10 @@
         <v>191</v>
       </c>
       <c r="H73">
-        <v>144254</v>
+        <v>144265</v>
       </c>
       <c r="I73">
-        <v>18319</v>
+        <v>18325</v>
       </c>
       <c r="J73" t="s">
         <v>221</v>
@@ -3601,10 +3601,10 @@
         <v>189</v>
       </c>
       <c r="H74">
-        <v>108947</v>
+        <v>108982</v>
       </c>
       <c r="I74">
-        <v>30873</v>
+        <v>30880</v>
       </c>
       <c r="J74" t="s">
         <v>207</v>
@@ -3636,10 +3636,10 @@
         <v>191</v>
       </c>
       <c r="H75">
-        <v>451018</v>
+        <v>451114</v>
       </c>
       <c r="I75">
-        <v>66011</v>
+        <v>66022</v>
       </c>
       <c r="J75" t="s">
         <v>208</v>
@@ -3671,10 +3671,10 @@
         <v>191</v>
       </c>
       <c r="H76">
-        <v>121325</v>
+        <v>121381</v>
       </c>
       <c r="I76">
-        <v>53056</v>
+        <v>53079</v>
       </c>
       <c r="J76" t="s">
         <v>205</v>
@@ -3706,10 +3706,10 @@
         <v>191</v>
       </c>
       <c r="H77">
-        <v>322492</v>
+        <v>322677</v>
       </c>
       <c r="I77">
-        <v>32343</v>
+        <v>32362</v>
       </c>
       <c r="J77" t="s">
         <v>222</v>
@@ -3741,10 +3741,10 @@
         <v>189</v>
       </c>
       <c r="H78">
-        <v>461929</v>
+        <v>462151</v>
       </c>
       <c r="I78">
-        <v>57516</v>
+        <v>57540</v>
       </c>
       <c r="J78" t="s">
         <v>223</v>
@@ -3776,10 +3776,10 @@
         <v>189</v>
       </c>
       <c r="H79">
-        <v>276711</v>
+        <v>276785</v>
       </c>
       <c r="I79">
-        <v>99165</v>
+        <v>99199</v>
       </c>
       <c r="J79" t="s">
         <v>224</v>
@@ -3846,10 +3846,10 @@
         <v>189</v>
       </c>
       <c r="H81">
-        <v>380283</v>
+        <v>380343</v>
       </c>
       <c r="I81">
-        <v>38661</v>
+        <v>38674</v>
       </c>
       <c r="J81" t="s">
         <v>198</v>
@@ -3881,10 +3881,10 @@
         <v>191</v>
       </c>
       <c r="H82">
-        <v>235867</v>
+        <v>235945</v>
       </c>
       <c r="I82">
-        <v>54323</v>
+        <v>54347</v>
       </c>
       <c r="J82" t="s">
         <v>225</v>
@@ -3916,10 +3916,10 @@
         <v>189</v>
       </c>
       <c r="H83">
-        <v>312191</v>
+        <v>312313</v>
       </c>
       <c r="I83">
-        <v>110410</v>
+        <v>110456</v>
       </c>
       <c r="J83" t="s">
         <v>197</v>
@@ -3951,10 +3951,10 @@
         <v>191</v>
       </c>
       <c r="H84">
-        <v>712107</v>
+        <v>712270</v>
       </c>
       <c r="I84">
-        <v>191859</v>
+        <v>191921</v>
       </c>
       <c r="J84" t="s">
         <v>226</v>
@@ -3986,10 +3986,10 @@
         <v>189</v>
       </c>
       <c r="H85">
-        <v>170158</v>
+        <v>170184</v>
       </c>
       <c r="I85">
-        <v>39823</v>
+        <v>39831</v>
       </c>
       <c r="J85" t="s">
         <v>197</v>
@@ -4021,10 +4021,10 @@
         <v>191</v>
       </c>
       <c r="H86">
-        <v>428365</v>
+        <v>428403</v>
       </c>
       <c r="I86">
-        <v>59038</v>
+        <v>59051</v>
       </c>
       <c r="J86" t="s">
         <v>208</v>
@@ -4056,10 +4056,10 @@
         <v>192</v>
       </c>
       <c r="H87">
-        <v>289120</v>
+        <v>289159</v>
       </c>
       <c r="I87">
-        <v>62044</v>
+        <v>62059</v>
       </c>
       <c r="J87" t="s">
         <v>227</v>
@@ -4091,10 +4091,10 @@
         <v>191</v>
       </c>
       <c r="H88">
-        <v>324943</v>
+        <v>325040</v>
       </c>
       <c r="I88">
-        <v>58366</v>
+        <v>58382</v>
       </c>
       <c r="J88" t="s">
         <v>228</v>
@@ -4126,10 +4126,10 @@
         <v>191</v>
       </c>
       <c r="H89">
-        <v>184118</v>
+        <v>184202</v>
       </c>
       <c r="I89">
-        <v>67621</v>
+        <v>67663</v>
       </c>
       <c r="J89" t="s">
         <v>205</v>
@@ -4161,10 +4161,10 @@
         <v>191</v>
       </c>
       <c r="H90">
-        <v>313671</v>
+        <v>313731</v>
       </c>
       <c r="I90">
-        <v>115655</v>
+        <v>115692</v>
       </c>
       <c r="J90" t="s">
         <v>229</v>
@@ -4196,10 +4196,10 @@
         <v>191</v>
       </c>
       <c r="H91">
-        <v>503209</v>
+        <v>503295</v>
       </c>
       <c r="I91">
-        <v>141069</v>
+        <v>141103</v>
       </c>
       <c r="J91" t="s">
         <v>208</v>
@@ -4231,10 +4231,10 @@
         <v>191</v>
       </c>
       <c r="H92">
-        <v>278826</v>
+        <v>278903</v>
       </c>
       <c r="I92">
-        <v>124793</v>
+        <v>124849</v>
       </c>
       <c r="J92" t="s">
         <v>208</v>
@@ -4266,10 +4266,10 @@
         <v>191</v>
       </c>
       <c r="H93">
-        <v>395439</v>
+        <v>395520</v>
       </c>
       <c r="I93">
-        <v>102364</v>
+        <v>102394</v>
       </c>
       <c r="J93" t="s">
         <v>230</v>
@@ -4301,10 +4301,10 @@
         <v>189</v>
       </c>
       <c r="H94">
-        <v>557091</v>
+        <v>557226</v>
       </c>
       <c r="I94">
-        <v>230361</v>
+        <v>230436</v>
       </c>
       <c r="J94" t="s">
         <v>231</v>
@@ -4336,10 +4336,10 @@
         <v>193</v>
       </c>
       <c r="H95">
-        <v>6447739</v>
+        <v>6448310</v>
       </c>
       <c r="I95">
-        <v>5327832</v>
+        <v>5328194</v>
       </c>
       <c r="J95" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
complted xlsx dash arrangement
</commit_message>
<xml_diff>
--- a/xlsx_data/codewars_stats_Filpill.xlsx
+++ b/xlsx_data/codewars_stats_Filpill.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -22,7 +23,7 @@
     <t>4 kyu</t>
   </si>
   <si>
-    <t>Filpill Codewars Stats since 12-Nov-2022</t>
+    <t>Filpill Codewars Stats since 13-Nov-2022</t>
   </si>
   <si>
     <t>Username</t>
@@ -736,7 +737,7 @@
     <t>white</t>
   </si>
   <si>
-    <t>Kata Compeleted By Filpill since 12-Nov-2022</t>
+    <t>Kata Compeleted By Filpill since 13-Nov-2022</t>
   </si>
   <si>
     <t>Kata ID</t>
@@ -854,7 +855,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill>
@@ -885,6 +886,163 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>303817</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>75973</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="monthly_complete.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11886217" cy="2742973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304422</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>37798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="language_pie.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2857500"/>
+          <a:ext cx="4571622" cy="3657298"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>243266</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>37798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="rank_distribution.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="2857500"/>
+          <a:ext cx="6948866" cy="3657298"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>608995</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="top_tags.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="0"/>
+          <a:ext cx="7314595" cy="6509990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1273,7 +1431,7 @@
         <v>1016</v>
       </c>
       <c r="D4">
-        <v>23252</v>
+        <v>23261</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1361,10 +1519,10 @@
         <v>189</v>
       </c>
       <c r="H10">
-        <v>491483</v>
+        <v>491722</v>
       </c>
       <c r="I10">
-        <v>28893</v>
+        <v>28913</v>
       </c>
       <c r="J10" t="s">
         <v>194</v>
@@ -1396,10 +1554,10 @@
         <v>189</v>
       </c>
       <c r="H11">
-        <v>401376</v>
+        <v>401463</v>
       </c>
       <c r="I11">
-        <v>53820</v>
+        <v>53834</v>
       </c>
       <c r="J11" t="s">
         <v>195</v>
@@ -1431,10 +1589,10 @@
         <v>190</v>
       </c>
       <c r="H12">
-        <v>84617</v>
+        <v>84647</v>
       </c>
       <c r="I12">
-        <v>5879</v>
+        <v>5881</v>
       </c>
       <c r="J12" t="s">
         <v>196</v>
@@ -1466,10 +1624,10 @@
         <v>189</v>
       </c>
       <c r="H13">
-        <v>311040</v>
+        <v>311076</v>
       </c>
       <c r="I13">
-        <v>41325</v>
+        <v>41343</v>
       </c>
       <c r="J13" t="s">
         <v>197</v>
@@ -1501,10 +1659,10 @@
         <v>189</v>
       </c>
       <c r="H14">
-        <v>288383</v>
+        <v>288506</v>
       </c>
       <c r="I14">
-        <v>45649</v>
+        <v>45666</v>
       </c>
       <c r="J14" t="s">
         <v>198</v>
@@ -1536,10 +1694,10 @@
         <v>191</v>
       </c>
       <c r="H15">
-        <v>182978</v>
+        <v>183042</v>
       </c>
       <c r="I15">
-        <v>49256</v>
+        <v>49273</v>
       </c>
       <c r="J15" t="s">
         <v>199</v>
@@ -1571,10 +1729,10 @@
         <v>189</v>
       </c>
       <c r="H16">
-        <v>182453</v>
+        <v>182523</v>
       </c>
       <c r="I16">
-        <v>50149</v>
+        <v>50168</v>
       </c>
       <c r="J16" t="s">
         <v>197</v>
@@ -1606,10 +1764,10 @@
         <v>191</v>
       </c>
       <c r="H17">
-        <v>383594</v>
+        <v>383722</v>
       </c>
       <c r="I17">
-        <v>52058</v>
+        <v>52082</v>
       </c>
       <c r="J17" t="s">
         <v>200</v>
@@ -1641,10 +1799,10 @@
         <v>191</v>
       </c>
       <c r="H18">
-        <v>223230</v>
+        <v>223268</v>
       </c>
       <c r="I18">
-        <v>58611</v>
+        <v>58626</v>
       </c>
       <c r="J18" t="s">
         <v>201</v>
@@ -1676,10 +1834,10 @@
         <v>189</v>
       </c>
       <c r="H19">
-        <v>228744</v>
+        <v>228857</v>
       </c>
       <c r="I19">
-        <v>59500</v>
+        <v>59544</v>
       </c>
       <c r="J19" t="s">
         <v>198</v>
@@ -1711,10 +1869,10 @@
         <v>191</v>
       </c>
       <c r="H20">
-        <v>322422</v>
+        <v>322478</v>
       </c>
       <c r="I20">
-        <v>64703</v>
+        <v>64730</v>
       </c>
       <c r="J20" t="s">
         <v>202</v>
@@ -1746,10 +1904,10 @@
         <v>189</v>
       </c>
       <c r="H21">
-        <v>338294</v>
+        <v>338394</v>
       </c>
       <c r="I21">
-        <v>87634</v>
+        <v>87676</v>
       </c>
       <c r="J21" t="s">
         <v>197</v>
@@ -1781,10 +1939,10 @@
         <v>189</v>
       </c>
       <c r="H22">
-        <v>535311</v>
+        <v>535628</v>
       </c>
       <c r="I22">
-        <v>89011</v>
+        <v>89050</v>
       </c>
       <c r="J22" t="s">
         <v>197</v>
@@ -1816,10 +1974,10 @@
         <v>189</v>
       </c>
       <c r="H23">
-        <v>479548</v>
+        <v>479726</v>
       </c>
       <c r="I23">
-        <v>114460</v>
+        <v>114514</v>
       </c>
       <c r="J23" t="s">
         <v>203</v>
@@ -1851,10 +2009,10 @@
         <v>189</v>
       </c>
       <c r="H24">
-        <v>634760</v>
+        <v>634952</v>
       </c>
       <c r="I24">
-        <v>115618</v>
+        <v>115657</v>
       </c>
       <c r="J24" t="s">
         <v>204</v>
@@ -1886,10 +2044,10 @@
         <v>189</v>
       </c>
       <c r="H25">
-        <v>48864</v>
+        <v>48884</v>
       </c>
       <c r="I25">
-        <v>14541</v>
+        <v>14548</v>
       </c>
       <c r="J25" t="s">
         <v>197</v>
@@ -1921,10 +2079,10 @@
         <v>191</v>
       </c>
       <c r="H26">
-        <v>677698</v>
+        <v>677879</v>
       </c>
       <c r="I26">
-        <v>163394</v>
+        <v>163455</v>
       </c>
       <c r="J26" t="s">
         <v>205</v>
@@ -1956,10 +2114,10 @@
         <v>189</v>
       </c>
       <c r="H27">
-        <v>431847</v>
+        <v>431985</v>
       </c>
       <c r="I27">
-        <v>175531</v>
+        <v>175593</v>
       </c>
       <c r="J27" t="s">
         <v>206</v>
@@ -1991,10 +2149,10 @@
         <v>189</v>
       </c>
       <c r="H28">
-        <v>701813</v>
+        <v>701975</v>
       </c>
       <c r="I28">
-        <v>191605</v>
+        <v>191679</v>
       </c>
       <c r="J28" t="s">
         <v>198</v>
@@ -2026,10 +2184,10 @@
         <v>189</v>
       </c>
       <c r="H29">
-        <v>785539</v>
+        <v>785732</v>
       </c>
       <c r="I29">
-        <v>197300</v>
+        <v>197360</v>
       </c>
       <c r="J29" t="s">
         <v>207</v>
@@ -2061,10 +2219,10 @@
         <v>191</v>
       </c>
       <c r="H30">
-        <v>634824</v>
+        <v>634944</v>
       </c>
       <c r="I30">
-        <v>215229</v>
+        <v>215290</v>
       </c>
       <c r="J30" t="s">
         <v>208</v>
@@ -2096,10 +2254,10 @@
         <v>191</v>
       </c>
       <c r="H31">
-        <v>725075</v>
+        <v>725274</v>
       </c>
       <c r="I31">
-        <v>233456</v>
+        <v>233537</v>
       </c>
       <c r="J31" t="s">
         <v>205</v>
@@ -2131,10 +2289,10 @@
         <v>189</v>
       </c>
       <c r="H32">
-        <v>884752</v>
+        <v>884932</v>
       </c>
       <c r="I32">
-        <v>295780</v>
+        <v>295861</v>
       </c>
       <c r="J32" t="s">
         <v>207</v>
@@ -2271,10 +2429,10 @@
         <v>191</v>
       </c>
       <c r="H36">
-        <v>27205</v>
+        <v>27207</v>
       </c>
       <c r="I36">
-        <v>6033</v>
+        <v>6034</v>
       </c>
       <c r="J36" t="s">
         <v>211</v>
@@ -2341,10 +2499,10 @@
         <v>191</v>
       </c>
       <c r="H38">
-        <v>13037</v>
+        <v>13038</v>
       </c>
       <c r="I38">
-        <v>2666</v>
+        <v>2667</v>
       </c>
       <c r="J38" t="s">
         <v>213</v>
@@ -2481,10 +2639,10 @@
         <v>191</v>
       </c>
       <c r="H42">
-        <v>36519</v>
+        <v>36522</v>
       </c>
       <c r="I42">
-        <v>5811</v>
+        <v>5813</v>
       </c>
       <c r="J42" t="s">
         <v>209</v>
@@ -2656,10 +2814,10 @@
         <v>191</v>
       </c>
       <c r="H47">
-        <v>51264</v>
+        <v>51268</v>
       </c>
       <c r="I47">
-        <v>9953</v>
+        <v>9954</v>
       </c>
       <c r="J47" t="s">
         <v>210</v>
@@ -2761,10 +2919,10 @@
         <v>191</v>
       </c>
       <c r="H50">
-        <v>43266</v>
+        <v>43275</v>
       </c>
       <c r="I50">
-        <v>10504</v>
+        <v>10506</v>
       </c>
       <c r="J50" t="s">
         <v>215</v>
@@ -2831,10 +2989,10 @@
         <v>191</v>
       </c>
       <c r="H52">
-        <v>62370</v>
+        <v>62374</v>
       </c>
       <c r="I52">
-        <v>10777</v>
+        <v>10778</v>
       </c>
       <c r="J52" t="s">
         <v>210</v>
@@ -2866,10 +3024,10 @@
         <v>191</v>
       </c>
       <c r="H53">
-        <v>37004</v>
+        <v>37010</v>
       </c>
       <c r="I53">
-        <v>15087</v>
+        <v>15088</v>
       </c>
       <c r="J53" t="s">
         <v>210</v>
@@ -2901,10 +3059,10 @@
         <v>191</v>
       </c>
       <c r="H54">
-        <v>40827</v>
+        <v>40829</v>
       </c>
       <c r="I54">
-        <v>6527</v>
+        <v>6529</v>
       </c>
       <c r="J54" t="s">
         <v>210</v>
@@ -2936,10 +3094,10 @@
         <v>191</v>
       </c>
       <c r="H55">
-        <v>30892</v>
+        <v>30893</v>
       </c>
       <c r="I55">
-        <v>2634</v>
+        <v>2635</v>
       </c>
       <c r="J55" t="s">
         <v>209</v>
@@ -2971,10 +3129,10 @@
         <v>191</v>
       </c>
       <c r="H56">
-        <v>37060</v>
+        <v>37068</v>
       </c>
       <c r="I56">
-        <v>8327</v>
+        <v>8329</v>
       </c>
       <c r="J56" t="s">
         <v>217</v>
@@ -3006,7 +3164,7 @@
         <v>191</v>
       </c>
       <c r="H57">
-        <v>19091</v>
+        <v>19093</v>
       </c>
       <c r="I57">
         <v>2214</v>
@@ -3076,10 +3234,10 @@
         <v>191</v>
       </c>
       <c r="H59">
-        <v>26986</v>
+        <v>26997</v>
       </c>
       <c r="I59">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J59" t="s">
         <v>209</v>
@@ -3111,10 +3269,10 @@
         <v>191</v>
       </c>
       <c r="H60">
-        <v>32526</v>
+        <v>32527</v>
       </c>
       <c r="I60">
-        <v>4734</v>
+        <v>4735</v>
       </c>
       <c r="J60" t="s">
         <v>219</v>
@@ -3146,10 +3304,10 @@
         <v>191</v>
       </c>
       <c r="H61">
-        <v>29129</v>
+        <v>29134</v>
       </c>
       <c r="I61">
-        <v>6053</v>
+        <v>6056</v>
       </c>
       <c r="J61" t="s">
         <v>210</v>
@@ -3181,10 +3339,10 @@
         <v>189</v>
       </c>
       <c r="H62">
-        <v>62831</v>
+        <v>62847</v>
       </c>
       <c r="I62">
-        <v>16448</v>
+        <v>16455</v>
       </c>
       <c r="J62" t="s">
         <v>197</v>
@@ -3216,7 +3374,7 @@
         <v>191</v>
       </c>
       <c r="H63">
-        <v>13294</v>
+        <v>13348</v>
       </c>
       <c r="I63">
         <v>1296</v>
@@ -3286,10 +3444,10 @@
         <v>191</v>
       </c>
       <c r="H65">
-        <v>34364</v>
+        <v>34370</v>
       </c>
       <c r="I65">
-        <v>3276</v>
+        <v>3277</v>
       </c>
       <c r="J65" t="s">
         <v>210</v>
@@ -3321,10 +3479,10 @@
         <v>191</v>
       </c>
       <c r="H66">
-        <v>73810</v>
+        <v>73816</v>
       </c>
       <c r="I66">
-        <v>8201</v>
+        <v>8204</v>
       </c>
       <c r="J66" t="s">
         <v>210</v>
@@ -3356,10 +3514,10 @@
         <v>191</v>
       </c>
       <c r="H67">
-        <v>28299</v>
+        <v>28314</v>
       </c>
       <c r="I67">
-        <v>6628</v>
+        <v>6631</v>
       </c>
       <c r="J67" t="s">
         <v>220</v>
@@ -3426,10 +3584,10 @@
         <v>191</v>
       </c>
       <c r="H69">
-        <v>52025</v>
+        <v>52027</v>
       </c>
       <c r="I69">
-        <v>10471</v>
+        <v>10472</v>
       </c>
       <c r="J69" t="s">
         <v>210</v>
@@ -3461,10 +3619,10 @@
         <v>189</v>
       </c>
       <c r="H70">
-        <v>183422</v>
+        <v>183484</v>
       </c>
       <c r="I70">
-        <v>15346</v>
+        <v>15352</v>
       </c>
       <c r="J70" t="s">
         <v>195</v>
@@ -3496,10 +3654,10 @@
         <v>191</v>
       </c>
       <c r="H71">
-        <v>85496</v>
+        <v>85500</v>
       </c>
       <c r="I71">
-        <v>7494</v>
+        <v>7496</v>
       </c>
       <c r="J71" t="s">
         <v>210</v>
@@ -3531,10 +3689,10 @@
         <v>191</v>
       </c>
       <c r="H72">
-        <v>58953</v>
+        <v>58966</v>
       </c>
       <c r="I72">
-        <v>15417</v>
+        <v>15424</v>
       </c>
       <c r="J72" t="s">
         <v>220</v>
@@ -3566,10 +3724,10 @@
         <v>191</v>
       </c>
       <c r="H73">
-        <v>144265</v>
+        <v>144276</v>
       </c>
       <c r="I73">
-        <v>18325</v>
+        <v>18329</v>
       </c>
       <c r="J73" t="s">
         <v>221</v>
@@ -3601,10 +3759,10 @@
         <v>189</v>
       </c>
       <c r="H74">
-        <v>108982</v>
+        <v>109003</v>
       </c>
       <c r="I74">
-        <v>30880</v>
+        <v>30890</v>
       </c>
       <c r="J74" t="s">
         <v>207</v>
@@ -3636,10 +3794,10 @@
         <v>191</v>
       </c>
       <c r="H75">
-        <v>451114</v>
+        <v>451194</v>
       </c>
       <c r="I75">
-        <v>66022</v>
+        <v>66039</v>
       </c>
       <c r="J75" t="s">
         <v>208</v>
@@ -3671,10 +3829,10 @@
         <v>191</v>
       </c>
       <c r="H76">
-        <v>121381</v>
+        <v>121448</v>
       </c>
       <c r="I76">
-        <v>53079</v>
+        <v>53104</v>
       </c>
       <c r="J76" t="s">
         <v>205</v>
@@ -3706,10 +3864,10 @@
         <v>191</v>
       </c>
       <c r="H77">
-        <v>322677</v>
+        <v>322783</v>
       </c>
       <c r="I77">
-        <v>32362</v>
+        <v>32378</v>
       </c>
       <c r="J77" t="s">
         <v>222</v>
@@ -3741,10 +3899,10 @@
         <v>189</v>
       </c>
       <c r="H78">
-        <v>462151</v>
+        <v>462362</v>
       </c>
       <c r="I78">
-        <v>57540</v>
+        <v>57574</v>
       </c>
       <c r="J78" t="s">
         <v>223</v>
@@ -3776,10 +3934,10 @@
         <v>189</v>
       </c>
       <c r="H79">
-        <v>276785</v>
+        <v>276844</v>
       </c>
       <c r="I79">
-        <v>99199</v>
+        <v>99230</v>
       </c>
       <c r="J79" t="s">
         <v>224</v>
@@ -3846,10 +4004,10 @@
         <v>189</v>
       </c>
       <c r="H81">
-        <v>380343</v>
+        <v>380394</v>
       </c>
       <c r="I81">
-        <v>38674</v>
+        <v>38682</v>
       </c>
       <c r="J81" t="s">
         <v>198</v>
@@ -3881,10 +4039,10 @@
         <v>191</v>
       </c>
       <c r="H82">
-        <v>235945</v>
+        <v>236023</v>
       </c>
       <c r="I82">
-        <v>54347</v>
+        <v>54366</v>
       </c>
       <c r="J82" t="s">
         <v>225</v>
@@ -3916,10 +4074,10 @@
         <v>189</v>
       </c>
       <c r="H83">
-        <v>312313</v>
+        <v>312416</v>
       </c>
       <c r="I83">
-        <v>110456</v>
+        <v>110515</v>
       </c>
       <c r="J83" t="s">
         <v>197</v>
@@ -3951,10 +4109,10 @@
         <v>191</v>
       </c>
       <c r="H84">
-        <v>712270</v>
+        <v>712529</v>
       </c>
       <c r="I84">
-        <v>191921</v>
+        <v>192008</v>
       </c>
       <c r="J84" t="s">
         <v>226</v>
@@ -3986,10 +4144,10 @@
         <v>189</v>
       </c>
       <c r="H85">
-        <v>170184</v>
+        <v>170211</v>
       </c>
       <c r="I85">
-        <v>39831</v>
+        <v>39844</v>
       </c>
       <c r="J85" t="s">
         <v>197</v>
@@ -4021,10 +4179,10 @@
         <v>191</v>
       </c>
       <c r="H86">
-        <v>428403</v>
+        <v>428461</v>
       </c>
       <c r="I86">
-        <v>59051</v>
+        <v>59066</v>
       </c>
       <c r="J86" t="s">
         <v>208</v>
@@ -4056,10 +4214,10 @@
         <v>192</v>
       </c>
       <c r="H87">
-        <v>289159</v>
+        <v>289232</v>
       </c>
       <c r="I87">
-        <v>62059</v>
+        <v>62073</v>
       </c>
       <c r="J87" t="s">
         <v>227</v>
@@ -4091,10 +4249,10 @@
         <v>191</v>
       </c>
       <c r="H88">
-        <v>325040</v>
+        <v>325186</v>
       </c>
       <c r="I88">
-        <v>58382</v>
+        <v>58400</v>
       </c>
       <c r="J88" t="s">
         <v>228</v>
@@ -4126,10 +4284,10 @@
         <v>191</v>
       </c>
       <c r="H89">
-        <v>184202</v>
+        <v>184345</v>
       </c>
       <c r="I89">
-        <v>67663</v>
+        <v>67715</v>
       </c>
       <c r="J89" t="s">
         <v>205</v>
@@ -4161,10 +4319,10 @@
         <v>191</v>
       </c>
       <c r="H90">
-        <v>313731</v>
+        <v>313806</v>
       </c>
       <c r="I90">
-        <v>115692</v>
+        <v>115737</v>
       </c>
       <c r="J90" t="s">
         <v>229</v>
@@ -4196,10 +4354,10 @@
         <v>191</v>
       </c>
       <c r="H91">
-        <v>503295</v>
+        <v>503481</v>
       </c>
       <c r="I91">
-        <v>141103</v>
+        <v>141153</v>
       </c>
       <c r="J91" t="s">
         <v>208</v>
@@ -4231,10 +4389,10 @@
         <v>191</v>
       </c>
       <c r="H92">
-        <v>278903</v>
+        <v>279015</v>
       </c>
       <c r="I92">
-        <v>124849</v>
+        <v>124913</v>
       </c>
       <c r="J92" t="s">
         <v>208</v>
@@ -4266,10 +4424,10 @@
         <v>191</v>
       </c>
       <c r="H93">
-        <v>395520</v>
+        <v>395604</v>
       </c>
       <c r="I93">
-        <v>102394</v>
+        <v>102423</v>
       </c>
       <c r="J93" t="s">
         <v>230</v>
@@ -4301,10 +4459,10 @@
         <v>189</v>
       </c>
       <c r="H94">
-        <v>557226</v>
+        <v>557394</v>
       </c>
       <c r="I94">
-        <v>230436</v>
+        <v>230519</v>
       </c>
       <c r="J94" t="s">
         <v>231</v>
@@ -4336,10 +4494,10 @@
         <v>193</v>
       </c>
       <c r="H95">
-        <v>6448310</v>
+        <v>6448854</v>
       </c>
       <c r="I95">
-        <v>5328194</v>
+        <v>5328604</v>
       </c>
       <c r="J95" t="s">
         <v>232</v>
@@ -4438,4 +4596,17 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
replaced streamlit local files with s3 links
</commit_message>
<xml_diff>
--- a/xlsx_data/codewars_stats_Filpill.xlsx
+++ b/xlsx_data/codewars_stats_Filpill.xlsx
@@ -3238,10 +3238,10 @@
         <v>702</v>
       </c>
       <c r="H10">
-        <v>76393</v>
+        <v>76410</v>
       </c>
       <c r="I10">
-        <v>10608</v>
+        <v>10613</v>
       </c>
       <c r="J10" t="s">
         <v>707</v>
@@ -3273,10 +3273,10 @@
         <v>702</v>
       </c>
       <c r="H11">
-        <v>120630</v>
+        <v>120641</v>
       </c>
       <c r="I11">
-        <v>10697</v>
+        <v>10700</v>
       </c>
       <c r="J11" t="s">
         <v>708</v>
@@ -3308,10 +3308,10 @@
         <v>703</v>
       </c>
       <c r="H12">
-        <v>140920</v>
+        <v>140970</v>
       </c>
       <c r="I12">
-        <v>25688</v>
+        <v>25706</v>
       </c>
       <c r="J12" t="s">
         <v>709</v>
@@ -3343,10 +3343,10 @@
         <v>704</v>
       </c>
       <c r="H13">
-        <v>198234</v>
+        <v>198266</v>
       </c>
       <c r="I13">
-        <v>22074</v>
+        <v>22082</v>
       </c>
       <c r="J13" t="s">
         <v>710</v>
@@ -3378,10 +3378,10 @@
         <v>702</v>
       </c>
       <c r="H14">
-        <v>220596</v>
+        <v>220643</v>
       </c>
       <c r="I14">
-        <v>37045</v>
+        <v>37052</v>
       </c>
       <c r="J14" t="s">
         <v>711</v>
@@ -3413,10 +3413,10 @@
         <v>702</v>
       </c>
       <c r="H15">
-        <v>278689</v>
+        <v>278790</v>
       </c>
       <c r="I15">
-        <v>39545</v>
+        <v>39567</v>
       </c>
       <c r="J15" t="s">
         <v>712</v>
@@ -3448,10 +3448,10 @@
         <v>702</v>
       </c>
       <c r="H16">
-        <v>286387</v>
+        <v>286461</v>
       </c>
       <c r="I16">
-        <v>40220</v>
+        <v>40231</v>
       </c>
       <c r="J16" t="s">
         <v>713</v>
@@ -3483,10 +3483,10 @@
         <v>702</v>
       </c>
       <c r="H17">
-        <v>918603</v>
+        <v>918667</v>
       </c>
       <c r="I17">
-        <v>90816</v>
+        <v>90831</v>
       </c>
       <c r="J17" t="s">
         <v>711</v>
@@ -3518,10 +3518,10 @@
         <v>702</v>
       </c>
       <c r="H18">
-        <v>308940</v>
+        <v>309027</v>
       </c>
       <c r="I18">
-        <v>100875</v>
+        <v>100915</v>
       </c>
       <c r="J18" t="s">
         <v>714</v>
@@ -3553,10 +3553,10 @@
         <v>702</v>
       </c>
       <c r="H19">
-        <v>577793</v>
+        <v>577965</v>
       </c>
       <c r="I19">
-        <v>129629</v>
+        <v>129668</v>
       </c>
       <c r="J19" t="s">
         <v>715</v>
@@ -3588,10 +3588,10 @@
         <v>702</v>
       </c>
       <c r="H20">
-        <v>588978</v>
+        <v>589080</v>
       </c>
       <c r="I20">
-        <v>161403</v>
+        <v>161439</v>
       </c>
       <c r="J20" t="s">
         <v>711</v>
@@ -3623,10 +3623,10 @@
         <v>704</v>
       </c>
       <c r="H21">
-        <v>159830</v>
+        <v>159862</v>
       </c>
       <c r="I21">
-        <v>47594</v>
+        <v>47613</v>
       </c>
       <c r="J21" t="s">
         <v>716</v>
@@ -3658,10 +3658,10 @@
         <v>704</v>
       </c>
       <c r="H22">
-        <v>49009</v>
+        <v>49023</v>
       </c>
       <c r="I22">
-        <v>20096</v>
+        <v>20102</v>
       </c>
       <c r="J22" t="s">
         <v>717</v>
@@ -3693,10 +3693,10 @@
         <v>704</v>
       </c>
       <c r="H23">
-        <v>48576</v>
+        <v>48595</v>
       </c>
       <c r="I23">
-        <v>21884</v>
+        <v>21897</v>
       </c>
       <c r="J23" t="s">
         <v>718</v>
@@ -3728,10 +3728,10 @@
         <v>704</v>
       </c>
       <c r="H24">
-        <v>56588</v>
+        <v>56596</v>
       </c>
       <c r="I24">
-        <v>20127</v>
+        <v>20133</v>
       </c>
       <c r="J24" t="s">
         <v>719</v>
@@ -3763,10 +3763,10 @@
         <v>704</v>
       </c>
       <c r="H25">
-        <v>63133</v>
+        <v>63218</v>
       </c>
       <c r="I25">
-        <v>24318</v>
+        <v>24350</v>
       </c>
       <c r="J25" t="s">
         <v>720</v>
@@ -3798,10 +3798,10 @@
         <v>704</v>
       </c>
       <c r="H26">
-        <v>51947</v>
+        <v>51968</v>
       </c>
       <c r="I26">
-        <v>21521</v>
+        <v>21527</v>
       </c>
       <c r="J26" t="s">
         <v>721</v>
@@ -3833,10 +3833,10 @@
         <v>704</v>
       </c>
       <c r="H27">
-        <v>48623</v>
+        <v>48629</v>
       </c>
       <c r="I27">
-        <v>18122</v>
+        <v>18126</v>
       </c>
       <c r="J27" t="s">
         <v>722</v>
@@ -3868,10 +3868,10 @@
         <v>704</v>
       </c>
       <c r="H28">
-        <v>29359</v>
+        <v>29368</v>
       </c>
       <c r="I28">
-        <v>15981</v>
+        <v>15986</v>
       </c>
       <c r="J28" t="s">
         <v>717</v>
@@ -3903,10 +3903,10 @@
         <v>704</v>
       </c>
       <c r="H29">
-        <v>64534</v>
+        <v>64566</v>
       </c>
       <c r="I29">
-        <v>34341</v>
+        <v>34363</v>
       </c>
       <c r="J29" t="s">
         <v>723</v>
@@ -3938,10 +3938,10 @@
         <v>704</v>
       </c>
       <c r="H30">
-        <v>193954</v>
+        <v>194089</v>
       </c>
       <c r="I30">
-        <v>87360</v>
+        <v>87432</v>
       </c>
       <c r="J30" t="s">
         <v>717</v>
@@ -3973,10 +3973,10 @@
         <v>704</v>
       </c>
       <c r="H31">
-        <v>120861</v>
+        <v>120867</v>
       </c>
       <c r="I31">
-        <v>22806</v>
+        <v>22808</v>
       </c>
       <c r="J31" t="s">
         <v>721</v>
@@ -4008,10 +4008,10 @@
         <v>704</v>
       </c>
       <c r="H32">
-        <v>189748</v>
+        <v>189858</v>
       </c>
       <c r="I32">
-        <v>84366</v>
+        <v>84428</v>
       </c>
       <c r="J32" t="s">
         <v>719</v>
@@ -4043,10 +4043,10 @@
         <v>704</v>
       </c>
       <c r="H33">
-        <v>51858</v>
+        <v>51870</v>
       </c>
       <c r="I33">
-        <v>24871</v>
+        <v>24879</v>
       </c>
       <c r="J33" t="s">
         <v>717</v>
@@ -4078,10 +4078,10 @@
         <v>704</v>
       </c>
       <c r="H34">
-        <v>183347</v>
+        <v>183360</v>
       </c>
       <c r="I34">
-        <v>22948</v>
+        <v>22951</v>
       </c>
       <c r="J34" t="s">
         <v>724</v>
@@ -4113,10 +4113,10 @@
         <v>704</v>
       </c>
       <c r="H35">
-        <v>112341</v>
+        <v>112367</v>
       </c>
       <c r="I35">
-        <v>34221</v>
+        <v>34232</v>
       </c>
       <c r="J35" t="s">
         <v>717</v>
@@ -4148,10 +4148,10 @@
         <v>704</v>
       </c>
       <c r="H36">
-        <v>548134</v>
+        <v>548199</v>
       </c>
       <c r="I36">
-        <v>170250</v>
+        <v>170291</v>
       </c>
       <c r="J36" t="s">
         <v>725</v>
@@ -4183,10 +4183,10 @@
         <v>704</v>
       </c>
       <c r="H37">
-        <v>471047</v>
+        <v>471156</v>
       </c>
       <c r="I37">
-        <v>185021</v>
+        <v>185073</v>
       </c>
       <c r="J37" t="s">
         <v>726</v>
@@ -4218,10 +4218,10 @@
         <v>704</v>
       </c>
       <c r="H38">
-        <v>72485</v>
+        <v>72504</v>
       </c>
       <c r="I38">
-        <v>26219</v>
+        <v>26228</v>
       </c>
       <c r="J38" t="s">
         <v>727</v>
@@ -4253,10 +4253,10 @@
         <v>704</v>
       </c>
       <c r="H39">
-        <v>67824</v>
+        <v>67851</v>
       </c>
       <c r="I39">
-        <v>23265</v>
+        <v>23283</v>
       </c>
       <c r="J39" t="s">
         <v>720</v>
@@ -4288,10 +4288,10 @@
         <v>704</v>
       </c>
       <c r="H40">
-        <v>65307</v>
+        <v>65311</v>
       </c>
       <c r="I40">
-        <v>20711</v>
+        <v>20714</v>
       </c>
       <c r="J40" t="s">
         <v>728</v>
@@ -4323,10 +4323,10 @@
         <v>704</v>
       </c>
       <c r="H41">
-        <v>60830</v>
+        <v>60846</v>
       </c>
       <c r="I41">
-        <v>15691</v>
+        <v>15698</v>
       </c>
       <c r="J41" t="s">
         <v>729</v>
@@ -4358,10 +4358,10 @@
         <v>704</v>
       </c>
       <c r="H42">
-        <v>65318</v>
+        <v>65327</v>
       </c>
       <c r="I42">
-        <v>16948</v>
+        <v>16952</v>
       </c>
       <c r="J42" t="s">
         <v>717</v>
@@ -4393,10 +4393,10 @@
         <v>704</v>
       </c>
       <c r="H43">
-        <v>68749</v>
+        <v>68770</v>
       </c>
       <c r="I43">
-        <v>25801</v>
+        <v>25807</v>
       </c>
       <c r="J43" t="s">
         <v>717</v>
@@ -4428,10 +4428,10 @@
         <v>704</v>
       </c>
       <c r="H44">
-        <v>181043</v>
+        <v>181094</v>
       </c>
       <c r="I44">
-        <v>86178</v>
+        <v>86212</v>
       </c>
       <c r="J44" t="s">
         <v>720</v>
@@ -4463,10 +4463,10 @@
         <v>704</v>
       </c>
       <c r="H45">
-        <v>262606</v>
+        <v>262654</v>
       </c>
       <c r="I45">
-        <v>101698</v>
+        <v>101732</v>
       </c>
       <c r="J45" t="s">
         <v>720</v>
@@ -4498,10 +4498,10 @@
         <v>704</v>
       </c>
       <c r="H46">
-        <v>388657</v>
+        <v>388774</v>
       </c>
       <c r="I46">
-        <v>92741</v>
+        <v>92773</v>
       </c>
       <c r="J46" t="s">
         <v>730</v>
@@ -4533,10 +4533,10 @@
         <v>704</v>
       </c>
       <c r="H47">
-        <v>39095</v>
+        <v>39106</v>
       </c>
       <c r="I47">
-        <v>23113</v>
+        <v>23119</v>
       </c>
       <c r="J47" t="s">
         <v>717</v>
@@ -4568,10 +4568,10 @@
         <v>704</v>
       </c>
       <c r="H48">
-        <v>74195</v>
+        <v>74206</v>
       </c>
       <c r="I48">
-        <v>28048</v>
+        <v>28055</v>
       </c>
       <c r="J48" t="s">
         <v>731</v>
@@ -4603,10 +4603,10 @@
         <v>704</v>
       </c>
       <c r="H49">
-        <v>90764</v>
+        <v>90799</v>
       </c>
       <c r="I49">
-        <v>30070</v>
+        <v>30083</v>
       </c>
       <c r="J49" t="s">
         <v>732</v>
@@ -4638,10 +4638,10 @@
         <v>704</v>
       </c>
       <c r="H50">
-        <v>45681</v>
+        <v>45686</v>
       </c>
       <c r="I50">
-        <v>20721</v>
+        <v>20726</v>
       </c>
       <c r="J50" t="s">
         <v>717</v>
@@ -4673,10 +4673,10 @@
         <v>704</v>
       </c>
       <c r="H51">
-        <v>43784</v>
+        <v>43792</v>
       </c>
       <c r="I51">
-        <v>23329</v>
+        <v>23337</v>
       </c>
       <c r="J51" t="s">
         <v>717</v>
@@ -4708,10 +4708,10 @@
         <v>704</v>
       </c>
       <c r="H52">
-        <v>98898</v>
+        <v>98917</v>
       </c>
       <c r="I52">
-        <v>34830</v>
+        <v>34833</v>
       </c>
       <c r="J52" t="s">
         <v>717</v>
@@ -4743,10 +4743,10 @@
         <v>704</v>
       </c>
       <c r="H53">
-        <v>61215</v>
+        <v>61233</v>
       </c>
       <c r="I53">
-        <v>19698</v>
+        <v>19708</v>
       </c>
       <c r="J53" t="s">
         <v>717</v>
@@ -4778,10 +4778,10 @@
         <v>704</v>
       </c>
       <c r="H54">
-        <v>52993</v>
+        <v>53000</v>
       </c>
       <c r="I54">
-        <v>19369</v>
+        <v>19373</v>
       </c>
       <c r="J54" t="s">
         <v>717</v>
@@ -4813,10 +4813,10 @@
         <v>704</v>
       </c>
       <c r="H55">
-        <v>320680</v>
+        <v>320859</v>
       </c>
       <c r="I55">
-        <v>120722</v>
+        <v>120786</v>
       </c>
       <c r="J55" t="s">
         <v>721</v>
@@ -4848,10 +4848,10 @@
         <v>704</v>
       </c>
       <c r="H56">
-        <v>196277</v>
+        <v>196420</v>
       </c>
       <c r="I56">
-        <v>85936</v>
+        <v>86015</v>
       </c>
       <c r="J56" t="s">
         <v>733</v>
@@ -4883,10 +4883,10 @@
         <v>704</v>
       </c>
       <c r="H57">
-        <v>32724</v>
+        <v>32739</v>
       </c>
       <c r="I57">
-        <v>17737</v>
+        <v>17748</v>
       </c>
       <c r="J57" t="s">
         <v>717</v>
@@ -4918,10 +4918,10 @@
         <v>702</v>
       </c>
       <c r="H58">
-        <v>173729</v>
+        <v>173800</v>
       </c>
       <c r="I58">
-        <v>35224</v>
+        <v>35237</v>
       </c>
       <c r="J58" t="s">
         <v>711</v>
@@ -4953,10 +4953,10 @@
         <v>702</v>
       </c>
       <c r="H59">
-        <v>118888</v>
+        <v>118964</v>
       </c>
       <c r="I59">
-        <v>18108</v>
+        <v>18121</v>
       </c>
       <c r="J59" t="s">
         <v>711</v>
@@ -4988,10 +4988,10 @@
         <v>704</v>
       </c>
       <c r="H60">
-        <v>79268</v>
+        <v>79298</v>
       </c>
       <c r="I60">
-        <v>22749</v>
+        <v>22757</v>
       </c>
       <c r="J60" t="s">
         <v>734</v>
@@ -5023,10 +5023,10 @@
         <v>704</v>
       </c>
       <c r="H61">
-        <v>321650</v>
+        <v>321754</v>
       </c>
       <c r="I61">
-        <v>157821</v>
+        <v>157900</v>
       </c>
       <c r="J61" t="s">
         <v>729</v>
@@ -5058,10 +5058,10 @@
         <v>704</v>
       </c>
       <c r="H62">
-        <v>90429</v>
+        <v>90455</v>
       </c>
       <c r="I62">
-        <v>41986</v>
+        <v>42005</v>
       </c>
       <c r="J62" t="s">
         <v>735</v>
@@ -5093,10 +5093,10 @@
         <v>704</v>
       </c>
       <c r="H63">
-        <v>122549</v>
+        <v>122630</v>
       </c>
       <c r="I63">
-        <v>39302</v>
+        <v>39328</v>
       </c>
       <c r="J63" t="s">
         <v>717</v>
@@ -5128,10 +5128,10 @@
         <v>704</v>
       </c>
       <c r="H64">
-        <v>102352</v>
+        <v>102413</v>
       </c>
       <c r="I64">
-        <v>43035</v>
+        <v>43069</v>
       </c>
       <c r="J64" t="s">
         <v>717</v>
@@ -5163,10 +5163,10 @@
         <v>704</v>
       </c>
       <c r="H65">
-        <v>109085</v>
+        <v>109112</v>
       </c>
       <c r="I65">
-        <v>26111</v>
+        <v>26116</v>
       </c>
       <c r="J65" t="s">
         <v>717</v>
@@ -5198,10 +5198,10 @@
         <v>704</v>
       </c>
       <c r="H66">
-        <v>29345</v>
+        <v>29366</v>
       </c>
       <c r="I66">
-        <v>22769</v>
+        <v>22788</v>
       </c>
       <c r="J66" t="s">
         <v>717</v>
@@ -5233,10 +5233,10 @@
         <v>704</v>
       </c>
       <c r="H67">
-        <v>326267</v>
+        <v>326422</v>
       </c>
       <c r="I67">
-        <v>162924</v>
+        <v>163007</v>
       </c>
       <c r="J67" t="s">
         <v>717</v>
@@ -5268,10 +5268,10 @@
         <v>704</v>
       </c>
       <c r="H68">
-        <v>288850</v>
+        <v>288929</v>
       </c>
       <c r="I68">
-        <v>74653</v>
+        <v>74681</v>
       </c>
       <c r="J68" t="s">
         <v>736</v>
@@ -5303,10 +5303,10 @@
         <v>704</v>
       </c>
       <c r="H69">
-        <v>71796</v>
+        <v>71807</v>
       </c>
       <c r="I69">
-        <v>26482</v>
+        <v>26490</v>
       </c>
       <c r="J69" t="s">
         <v>735</v>
@@ -5338,10 +5338,10 @@
         <v>704</v>
       </c>
       <c r="H70">
-        <v>62337</v>
+        <v>62365</v>
       </c>
       <c r="I70">
-        <v>22392</v>
+        <v>22398</v>
       </c>
       <c r="J70" t="s">
         <v>717</v>
@@ -5373,10 +5373,10 @@
         <v>704</v>
       </c>
       <c r="H71">
-        <v>51355</v>
+        <v>51381</v>
       </c>
       <c r="I71">
-        <v>18824</v>
+        <v>18836</v>
       </c>
       <c r="J71" t="s">
         <v>717</v>
@@ -5408,10 +5408,10 @@
         <v>704</v>
       </c>
       <c r="H72">
-        <v>665206</v>
+        <v>665392</v>
       </c>
       <c r="I72">
-        <v>158902</v>
+        <v>158940</v>
       </c>
       <c r="J72" t="s">
         <v>727</v>
@@ -5443,10 +5443,10 @@
         <v>704</v>
       </c>
       <c r="H73">
-        <v>112360</v>
+        <v>112411</v>
       </c>
       <c r="I73">
-        <v>54760</v>
+        <v>54793</v>
       </c>
       <c r="J73" t="s">
         <v>721</v>
@@ -5478,10 +5478,10 @@
         <v>704</v>
       </c>
       <c r="H74">
-        <v>64270</v>
+        <v>64299</v>
       </c>
       <c r="I74">
-        <v>32808</v>
+        <v>32826</v>
       </c>
       <c r="J74" t="s">
         <v>729</v>
@@ -5513,10 +5513,10 @@
         <v>704</v>
       </c>
       <c r="H75">
-        <v>74086</v>
+        <v>74116</v>
       </c>
       <c r="I75">
-        <v>18939</v>
+        <v>18946</v>
       </c>
       <c r="J75" t="s">
         <v>729</v>
@@ -5548,10 +5548,10 @@
         <v>704</v>
       </c>
       <c r="H76">
-        <v>84205</v>
+        <v>84256</v>
       </c>
       <c r="I76">
-        <v>34742</v>
+        <v>34758</v>
       </c>
       <c r="J76" t="s">
         <v>737</v>
@@ -5583,10 +5583,10 @@
         <v>704</v>
       </c>
       <c r="H77">
-        <v>229808</v>
+        <v>229898</v>
       </c>
       <c r="I77">
-        <v>120355</v>
+        <v>120419</v>
       </c>
       <c r="J77" t="s">
         <v>737</v>
@@ -5618,10 +5618,10 @@
         <v>704</v>
       </c>
       <c r="H78">
-        <v>41713</v>
+        <v>41764</v>
       </c>
       <c r="I78">
-        <v>20923</v>
+        <v>20957</v>
       </c>
       <c r="J78" t="s">
         <v>738</v>
@@ -5653,10 +5653,10 @@
         <v>704</v>
       </c>
       <c r="H79">
-        <v>128107</v>
+        <v>128137</v>
       </c>
       <c r="I79">
-        <v>40432</v>
+        <v>40446</v>
       </c>
       <c r="J79" t="s">
         <v>721</v>
@@ -5688,10 +5688,10 @@
         <v>704</v>
       </c>
       <c r="H80">
-        <v>50229</v>
+        <v>50247</v>
       </c>
       <c r="I80">
-        <v>28013</v>
+        <v>28029</v>
       </c>
       <c r="J80" t="s">
         <v>739</v>
@@ -5723,10 +5723,10 @@
         <v>704</v>
       </c>
       <c r="H81">
-        <v>154458</v>
+        <v>154544</v>
       </c>
       <c r="I81">
-        <v>78960</v>
+        <v>79018</v>
       </c>
       <c r="J81" t="s">
         <v>740</v>
@@ -5758,10 +5758,10 @@
         <v>704</v>
       </c>
       <c r="H82">
-        <v>62551</v>
+        <v>62593</v>
       </c>
       <c r="I82">
-        <v>36981</v>
+        <v>37017</v>
       </c>
       <c r="J82" t="s">
         <v>717</v>
@@ -5793,10 +5793,10 @@
         <v>704</v>
       </c>
       <c r="H83">
-        <v>104248</v>
+        <v>104285</v>
       </c>
       <c r="I83">
-        <v>31842</v>
+        <v>31858</v>
       </c>
       <c r="J83" t="s">
         <v>719</v>
@@ -5828,10 +5828,10 @@
         <v>702</v>
       </c>
       <c r="H84">
-        <v>224449</v>
+        <v>224520</v>
       </c>
       <c r="I84">
-        <v>27302</v>
+        <v>27312</v>
       </c>
       <c r="J84" t="s">
         <v>741</v>
@@ -5863,10 +5863,10 @@
         <v>702</v>
       </c>
       <c r="H85">
-        <v>156504</v>
+        <v>156566</v>
       </c>
       <c r="I85">
-        <v>35129</v>
+        <v>35138</v>
       </c>
       <c r="J85" t="s">
         <v>742</v>
@@ -5898,10 +5898,10 @@
         <v>702</v>
       </c>
       <c r="H86">
-        <v>126010</v>
+        <v>126063</v>
       </c>
       <c r="I86">
-        <v>26144</v>
+        <v>26151</v>
       </c>
       <c r="J86" t="s">
         <v>711</v>
@@ -5968,7 +5968,7 @@
         <v>702</v>
       </c>
       <c r="H88">
-        <v>29843</v>
+        <v>29856</v>
       </c>
       <c r="I88">
         <v>929</v>
@@ -6003,10 +6003,10 @@
         <v>704</v>
       </c>
       <c r="H89">
-        <v>24762</v>
+        <v>24766</v>
       </c>
       <c r="I89">
-        <v>5711</v>
+        <v>5712</v>
       </c>
       <c r="J89" t="s">
         <v>745</v>
@@ -6038,10 +6038,10 @@
         <v>704</v>
       </c>
       <c r="H90">
-        <v>63717</v>
+        <v>63724</v>
       </c>
       <c r="I90">
-        <v>17303</v>
+        <v>17306</v>
       </c>
       <c r="J90" t="s">
         <v>746</v>
@@ -6108,10 +6108,10 @@
         <v>704</v>
       </c>
       <c r="H92">
-        <v>42130</v>
+        <v>42144</v>
       </c>
       <c r="I92">
-        <v>18098</v>
+        <v>18104</v>
       </c>
       <c r="J92" t="s">
         <v>748</v>
@@ -6143,10 +6143,10 @@
         <v>704</v>
       </c>
       <c r="H93">
-        <v>22590</v>
+        <v>22602</v>
       </c>
       <c r="I93">
-        <v>8999</v>
+        <v>9003</v>
       </c>
       <c r="J93" t="s">
         <v>747</v>
@@ -6178,10 +6178,10 @@
         <v>704</v>
       </c>
       <c r="H94">
-        <v>22100</v>
+        <v>22105</v>
       </c>
       <c r="I94">
-        <v>8445</v>
+        <v>8446</v>
       </c>
       <c r="J94" t="s">
         <v>747</v>
@@ -6213,7 +6213,7 @@
         <v>704</v>
       </c>
       <c r="H95">
-        <v>10957</v>
+        <v>10966</v>
       </c>
       <c r="I95">
         <v>1993</v>
@@ -6248,10 +6248,10 @@
         <v>704</v>
       </c>
       <c r="H96">
-        <v>27458</v>
+        <v>27478</v>
       </c>
       <c r="I96">
-        <v>4550</v>
+        <v>4553</v>
       </c>
       <c r="J96" t="s">
         <v>749</v>
@@ -6283,7 +6283,7 @@
         <v>704</v>
       </c>
       <c r="H97">
-        <v>24766</v>
+        <v>24769</v>
       </c>
       <c r="I97">
         <v>5595</v>
@@ -6353,10 +6353,10 @@
         <v>704</v>
       </c>
       <c r="H99">
-        <v>29707</v>
+        <v>29709</v>
       </c>
       <c r="I99">
-        <v>10769</v>
+        <v>10771</v>
       </c>
       <c r="J99" t="s">
         <v>750</v>
@@ -6388,10 +6388,10 @@
         <v>704</v>
       </c>
       <c r="H100">
-        <v>29453</v>
+        <v>29458</v>
       </c>
       <c r="I100">
-        <v>11787</v>
+        <v>11789</v>
       </c>
       <c r="J100" t="s">
         <v>747</v>
@@ -6423,10 +6423,10 @@
         <v>704</v>
       </c>
       <c r="H101">
-        <v>11737</v>
+        <v>11738</v>
       </c>
       <c r="I101">
-        <v>5138</v>
+        <v>5139</v>
       </c>
       <c r="J101" t="s">
         <v>750</v>
@@ -6458,10 +6458,10 @@
         <v>704</v>
       </c>
       <c r="H102">
-        <v>12184</v>
+        <v>12198</v>
       </c>
       <c r="I102">
-        <v>2711</v>
+        <v>2712</v>
       </c>
       <c r="J102" t="s">
         <v>750</v>
@@ -6493,10 +6493,10 @@
         <v>704</v>
       </c>
       <c r="H103">
-        <v>27246</v>
+        <v>27255</v>
       </c>
       <c r="I103">
-        <v>5671</v>
+        <v>5672</v>
       </c>
       <c r="J103" t="s">
         <v>751</v>
@@ -6598,10 +6598,10 @@
         <v>704</v>
       </c>
       <c r="H106">
-        <v>34083</v>
+        <v>34085</v>
       </c>
       <c r="I106">
-        <v>8456</v>
+        <v>8457</v>
       </c>
       <c r="J106" t="s">
         <v>752</v>
@@ -6633,10 +6633,10 @@
         <v>704</v>
       </c>
       <c r="H107">
-        <v>19308</v>
+        <v>19312</v>
       </c>
       <c r="I107">
-        <v>6748</v>
+        <v>6749</v>
       </c>
       <c r="J107" t="s">
         <v>750</v>
@@ -6668,10 +6668,10 @@
         <v>704</v>
       </c>
       <c r="H108">
-        <v>19451</v>
+        <v>19454</v>
       </c>
       <c r="I108">
-        <v>4992</v>
+        <v>4993</v>
       </c>
       <c r="J108" t="s">
         <v>752</v>
@@ -6738,10 +6738,10 @@
         <v>704</v>
       </c>
       <c r="H110">
-        <v>22405</v>
+        <v>22406</v>
       </c>
       <c r="I110">
-        <v>6362</v>
+        <v>6363</v>
       </c>
       <c r="J110" t="s">
         <v>748</v>
@@ -6773,7 +6773,7 @@
         <v>704</v>
       </c>
       <c r="H111">
-        <v>37727</v>
+        <v>37734</v>
       </c>
       <c r="I111">
         <v>5853</v>
@@ -6808,10 +6808,10 @@
         <v>704</v>
       </c>
       <c r="H112">
-        <v>30745</v>
+        <v>30748</v>
       </c>
       <c r="I112">
-        <v>7167</v>
+        <v>7169</v>
       </c>
       <c r="J112" t="s">
         <v>753</v>
@@ -6843,10 +6843,10 @@
         <v>704</v>
       </c>
       <c r="H113">
-        <v>61237</v>
+        <v>61255</v>
       </c>
       <c r="I113">
-        <v>6989</v>
+        <v>6990</v>
       </c>
       <c r="J113" t="s">
         <v>753</v>
@@ -6878,7 +6878,7 @@
         <v>704</v>
       </c>
       <c r="H114">
-        <v>35575</v>
+        <v>35576</v>
       </c>
       <c r="I114">
         <v>7513</v>
@@ -6913,10 +6913,10 @@
         <v>704</v>
       </c>
       <c r="H115">
-        <v>34337</v>
+        <v>34341</v>
       </c>
       <c r="I115">
-        <v>18231</v>
+        <v>18234</v>
       </c>
       <c r="J115" t="s">
         <v>754</v>
@@ -6948,10 +6948,10 @@
         <v>702</v>
       </c>
       <c r="H116">
-        <v>33283</v>
+        <v>33285</v>
       </c>
       <c r="I116">
-        <v>11090</v>
+        <v>11091</v>
       </c>
       <c r="J116" t="s">
         <v>755</v>
@@ -6983,10 +6983,10 @@
         <v>704</v>
       </c>
       <c r="H117">
-        <v>25969</v>
+        <v>25980</v>
       </c>
       <c r="I117">
-        <v>15905</v>
+        <v>15909</v>
       </c>
       <c r="J117" t="s">
         <v>745</v>
@@ -7018,10 +7018,10 @@
         <v>704</v>
       </c>
       <c r="H118">
-        <v>33997</v>
+        <v>34010</v>
       </c>
       <c r="I118">
-        <v>15504</v>
+        <v>15510</v>
       </c>
       <c r="J118" t="s">
         <v>745</v>
@@ -7053,10 +7053,10 @@
         <v>704</v>
       </c>
       <c r="H119">
-        <v>23417</v>
+        <v>23421</v>
       </c>
       <c r="I119">
-        <v>16920</v>
+        <v>16924</v>
       </c>
       <c r="J119" t="s">
         <v>745</v>
@@ -7088,10 +7088,10 @@
         <v>704</v>
       </c>
       <c r="H120">
-        <v>21554</v>
+        <v>21558</v>
       </c>
       <c r="I120">
-        <v>14647</v>
+        <v>14650</v>
       </c>
       <c r="J120" t="s">
         <v>745</v>
@@ -7123,10 +7123,10 @@
         <v>704</v>
       </c>
       <c r="H121">
-        <v>38165</v>
+        <v>38171</v>
       </c>
       <c r="I121">
-        <v>23683</v>
+        <v>23688</v>
       </c>
       <c r="J121" t="s">
         <v>753</v>
@@ -7158,10 +7158,10 @@
         <v>704</v>
       </c>
       <c r="H122">
-        <v>42983</v>
+        <v>42989</v>
       </c>
       <c r="I122">
-        <v>19045</v>
+        <v>19050</v>
       </c>
       <c r="J122" t="s">
         <v>753</v>
@@ -7193,10 +7193,10 @@
         <v>704</v>
       </c>
       <c r="H123">
-        <v>36802</v>
+        <v>36809</v>
       </c>
       <c r="I123">
-        <v>15504</v>
+        <v>15509</v>
       </c>
       <c r="J123" t="s">
         <v>748</v>
@@ -7228,10 +7228,10 @@
         <v>704</v>
       </c>
       <c r="H124">
-        <v>28531</v>
+        <v>28536</v>
       </c>
       <c r="I124">
-        <v>17121</v>
+        <v>17126</v>
       </c>
       <c r="J124" t="s">
         <v>748</v>
@@ -7263,10 +7263,10 @@
         <v>704</v>
       </c>
       <c r="H125">
-        <v>23021</v>
+        <v>23024</v>
       </c>
       <c r="I125">
-        <v>14988</v>
+        <v>14991</v>
       </c>
       <c r="J125" t="s">
         <v>747</v>
@@ -7298,10 +7298,10 @@
         <v>704</v>
       </c>
       <c r="H126">
-        <v>27860</v>
+        <v>27866</v>
       </c>
       <c r="I126">
-        <v>11663</v>
+        <v>11665</v>
       </c>
       <c r="J126" t="s">
         <v>750</v>
@@ -7333,10 +7333,10 @@
         <v>704</v>
       </c>
       <c r="H127">
-        <v>23633</v>
+        <v>23634</v>
       </c>
       <c r="I127">
-        <v>7258</v>
+        <v>7259</v>
       </c>
       <c r="J127" t="s">
         <v>747</v>
@@ -7368,10 +7368,10 @@
         <v>704</v>
       </c>
       <c r="H128">
-        <v>30191</v>
+        <v>30192</v>
       </c>
       <c r="I128">
-        <v>10092</v>
+        <v>10093</v>
       </c>
       <c r="J128" t="s">
         <v>747</v>
@@ -7403,10 +7403,10 @@
         <v>704</v>
       </c>
       <c r="H129">
-        <v>16838</v>
+        <v>16839</v>
       </c>
       <c r="I129">
-        <v>6641</v>
+        <v>6642</v>
       </c>
       <c r="J129" t="s">
         <v>751</v>
@@ -7438,10 +7438,10 @@
         <v>704</v>
       </c>
       <c r="H130">
-        <v>24672</v>
+        <v>24675</v>
       </c>
       <c r="I130">
-        <v>7996</v>
+        <v>7998</v>
       </c>
       <c r="J130" t="s">
         <v>748</v>
@@ -7508,10 +7508,10 @@
         <v>704</v>
       </c>
       <c r="H132">
-        <v>40936</v>
+        <v>41010</v>
       </c>
       <c r="I132">
-        <v>17872</v>
+        <v>17876</v>
       </c>
       <c r="J132" t="s">
         <v>745</v>
@@ -7543,10 +7543,10 @@
         <v>704</v>
       </c>
       <c r="H133">
-        <v>25825</v>
+        <v>25843</v>
       </c>
       <c r="I133">
-        <v>6403</v>
+        <v>6405</v>
       </c>
       <c r="J133" t="s">
         <v>747</v>
@@ -7578,10 +7578,10 @@
         <v>704</v>
       </c>
       <c r="H134">
-        <v>33618</v>
+        <v>33620</v>
       </c>
       <c r="I134">
-        <v>5697</v>
+        <v>5698</v>
       </c>
       <c r="J134" t="s">
         <v>751</v>
@@ -7683,10 +7683,10 @@
         <v>704</v>
       </c>
       <c r="H137">
-        <v>21549</v>
+        <v>21553</v>
       </c>
       <c r="I137">
-        <v>12232</v>
+        <v>12234</v>
       </c>
       <c r="J137" t="s">
         <v>751</v>
@@ -7718,10 +7718,10 @@
         <v>704</v>
       </c>
       <c r="H138">
-        <v>116370</v>
+        <v>116436</v>
       </c>
       <c r="I138">
-        <v>77903</v>
+        <v>77962</v>
       </c>
       <c r="J138" t="s">
         <v>717</v>
@@ -7753,10 +7753,10 @@
         <v>704</v>
       </c>
       <c r="H139">
-        <v>243870</v>
+        <v>243911</v>
       </c>
       <c r="I139">
-        <v>69840</v>
+        <v>69863</v>
       </c>
       <c r="J139" t="s">
         <v>756</v>
@@ -7788,10 +7788,10 @@
         <v>704</v>
       </c>
       <c r="H140">
-        <v>46331</v>
+        <v>46343</v>
       </c>
       <c r="I140">
-        <v>24475</v>
+        <v>24485</v>
       </c>
       <c r="J140" t="s">
         <v>719</v>
@@ -7823,10 +7823,10 @@
         <v>704</v>
       </c>
       <c r="H141">
-        <v>338486</v>
+        <v>338608</v>
       </c>
       <c r="I141">
-        <v>65888</v>
+        <v>65907</v>
       </c>
       <c r="J141" t="s">
         <v>757</v>
@@ -7858,10 +7858,10 @@
         <v>704</v>
       </c>
       <c r="H142">
-        <v>43630</v>
+        <v>43633</v>
       </c>
       <c r="I142">
-        <v>10452</v>
+        <v>10455</v>
       </c>
       <c r="J142" t="s">
         <v>717</v>
@@ -7893,10 +7893,10 @@
         <v>704</v>
       </c>
       <c r="H143">
-        <v>464541</v>
+        <v>464668</v>
       </c>
       <c r="I143">
-        <v>116471</v>
+        <v>116515</v>
       </c>
       <c r="J143" t="s">
         <v>758</v>
@@ -7928,10 +7928,10 @@
         <v>704</v>
       </c>
       <c r="H144">
-        <v>167136</v>
+        <v>167233</v>
       </c>
       <c r="I144">
-        <v>33787</v>
+        <v>33807</v>
       </c>
       <c r="J144" t="s">
         <v>717</v>
@@ -7963,10 +7963,10 @@
         <v>704</v>
       </c>
       <c r="H145">
-        <v>125537</v>
+        <v>125585</v>
       </c>
       <c r="I145">
-        <v>32038</v>
+        <v>32055</v>
       </c>
       <c r="J145" t="s">
         <v>717</v>
@@ -7998,10 +7998,10 @@
         <v>704</v>
       </c>
       <c r="H146">
-        <v>97028</v>
+        <v>97083</v>
       </c>
       <c r="I146">
-        <v>48036</v>
+        <v>48062</v>
       </c>
       <c r="J146" t="s">
         <v>729</v>
@@ -8033,10 +8033,10 @@
         <v>704</v>
       </c>
       <c r="H147">
-        <v>99843</v>
+        <v>99874</v>
       </c>
       <c r="I147">
-        <v>46586</v>
+        <v>46608</v>
       </c>
       <c r="J147" t="s">
         <v>759</v>
@@ -8068,10 +8068,10 @@
         <v>704</v>
       </c>
       <c r="H148">
-        <v>61234</v>
+        <v>61270</v>
       </c>
       <c r="I148">
-        <v>38780</v>
+        <v>38805</v>
       </c>
       <c r="J148" t="s">
         <v>717</v>
@@ -8103,10 +8103,10 @@
         <v>704</v>
       </c>
       <c r="H149">
-        <v>92343</v>
+        <v>92359</v>
       </c>
       <c r="I149">
-        <v>30709</v>
+        <v>30714</v>
       </c>
       <c r="J149" t="s">
         <v>760</v>
@@ -8138,10 +8138,10 @@
         <v>704</v>
       </c>
       <c r="H150">
-        <v>64275</v>
+        <v>64298</v>
       </c>
       <c r="I150">
-        <v>27257</v>
+        <v>27271</v>
       </c>
       <c r="J150" t="s">
         <v>735</v>
@@ -8173,10 +8173,10 @@
         <v>704</v>
       </c>
       <c r="H151">
-        <v>86765</v>
+        <v>86827</v>
       </c>
       <c r="I151">
-        <v>31421</v>
+        <v>31451</v>
       </c>
       <c r="J151" t="s">
         <v>717</v>
@@ -8208,10 +8208,10 @@
         <v>704</v>
       </c>
       <c r="H152">
-        <v>98428</v>
+        <v>98453</v>
       </c>
       <c r="I152">
-        <v>31609</v>
+        <v>31620</v>
       </c>
       <c r="J152" t="s">
         <v>717</v>
@@ -8243,10 +8243,10 @@
         <v>704</v>
       </c>
       <c r="H153">
-        <v>178438</v>
+        <v>178548</v>
       </c>
       <c r="I153">
-        <v>74940</v>
+        <v>75008</v>
       </c>
       <c r="J153" t="s">
         <v>717</v>
@@ -8278,10 +8278,10 @@
         <v>704</v>
       </c>
       <c r="H154">
-        <v>212787</v>
+        <v>212905</v>
       </c>
       <c r="I154">
-        <v>121318</v>
+        <v>121396</v>
       </c>
       <c r="J154" t="s">
         <v>719</v>
@@ -8313,10 +8313,10 @@
         <v>704</v>
       </c>
       <c r="H155">
-        <v>94515</v>
+        <v>94578</v>
       </c>
       <c r="I155">
-        <v>45799</v>
+        <v>45836</v>
       </c>
       <c r="J155" t="s">
         <v>717</v>
@@ -8348,10 +8348,10 @@
         <v>704</v>
       </c>
       <c r="H156">
-        <v>717428</v>
+        <v>717617</v>
       </c>
       <c r="I156">
-        <v>240748</v>
+        <v>240834</v>
       </c>
       <c r="J156" t="s">
         <v>761</v>
@@ -8383,10 +8383,10 @@
         <v>704</v>
       </c>
       <c r="H157">
-        <v>65797</v>
+        <v>65826</v>
       </c>
       <c r="I157">
-        <v>36478</v>
+        <v>36496</v>
       </c>
       <c r="J157" t="s">
         <v>717</v>
@@ -8418,10 +8418,10 @@
         <v>704</v>
       </c>
       <c r="H158">
-        <v>153768</v>
+        <v>153805</v>
       </c>
       <c r="I158">
-        <v>33396</v>
+        <v>33410</v>
       </c>
       <c r="J158" t="s">
         <v>735</v>
@@ -8453,10 +8453,10 @@
         <v>704</v>
       </c>
       <c r="H159">
-        <v>709203</v>
+        <v>709485</v>
       </c>
       <c r="I159">
-        <v>122216</v>
+        <v>122247</v>
       </c>
       <c r="J159" t="s">
         <v>717</v>
@@ -8488,10 +8488,10 @@
         <v>704</v>
       </c>
       <c r="H160">
-        <v>293584</v>
+        <v>293654</v>
       </c>
       <c r="I160">
-        <v>114233</v>
+        <v>114270</v>
       </c>
       <c r="J160" t="s">
         <v>717</v>
@@ -8523,10 +8523,10 @@
         <v>704</v>
       </c>
       <c r="H161">
-        <v>184317</v>
+        <v>184344</v>
       </c>
       <c r="I161">
-        <v>42151</v>
+        <v>42160</v>
       </c>
       <c r="J161" t="s">
         <v>723</v>
@@ -8558,10 +8558,10 @@
         <v>704</v>
       </c>
       <c r="H162">
-        <v>61639</v>
+        <v>61722</v>
       </c>
       <c r="I162">
-        <v>27072</v>
+        <v>27082</v>
       </c>
       <c r="J162" t="s">
         <v>762</v>
@@ -8593,10 +8593,10 @@
         <v>704</v>
       </c>
       <c r="H163">
-        <v>134205</v>
+        <v>134268</v>
       </c>
       <c r="I163">
-        <v>38285</v>
+        <v>38306</v>
       </c>
       <c r="J163" t="s">
         <v>729</v>
@@ -8628,10 +8628,10 @@
         <v>704</v>
       </c>
       <c r="H164">
-        <v>142488</v>
+        <v>142578</v>
       </c>
       <c r="I164">
-        <v>59637</v>
+        <v>59682</v>
       </c>
       <c r="J164" t="s">
         <v>717</v>
@@ -8663,10 +8663,10 @@
         <v>704</v>
       </c>
       <c r="H165">
-        <v>92329</v>
+        <v>92465</v>
       </c>
       <c r="I165">
-        <v>43926</v>
+        <v>43963</v>
       </c>
       <c r="J165" t="s">
         <v>721</v>
@@ -8698,10 +8698,10 @@
         <v>704</v>
       </c>
       <c r="H166">
-        <v>107616</v>
+        <v>107640</v>
       </c>
       <c r="I166">
-        <v>37810</v>
+        <v>37823</v>
       </c>
       <c r="J166" t="s">
         <v>763</v>
@@ -8733,10 +8733,10 @@
         <v>704</v>
       </c>
       <c r="H167">
-        <v>71865</v>
+        <v>71890</v>
       </c>
       <c r="I167">
-        <v>32792</v>
+        <v>32809</v>
       </c>
       <c r="J167" t="s">
         <v>717</v>
@@ -8768,10 +8768,10 @@
         <v>704</v>
       </c>
       <c r="H168">
-        <v>80850</v>
+        <v>80881</v>
       </c>
       <c r="I168">
-        <v>59074</v>
+        <v>59101</v>
       </c>
       <c r="J168" t="s">
         <v>764</v>
@@ -8803,10 +8803,10 @@
         <v>704</v>
       </c>
       <c r="H169">
-        <v>88218</v>
+        <v>88246</v>
       </c>
       <c r="I169">
-        <v>34075</v>
+        <v>34094</v>
       </c>
       <c r="J169" t="s">
         <v>729</v>
@@ -8838,10 +8838,10 @@
         <v>704</v>
       </c>
       <c r="H170">
-        <v>299594</v>
+        <v>299648</v>
       </c>
       <c r="I170">
-        <v>117037</v>
+        <v>117068</v>
       </c>
       <c r="J170" t="s">
         <v>765</v>
@@ -8873,10 +8873,10 @@
         <v>704</v>
       </c>
       <c r="H171">
-        <v>736563</v>
+        <v>736991</v>
       </c>
       <c r="I171">
-        <v>211960</v>
+        <v>212113</v>
       </c>
       <c r="J171" t="s">
         <v>729</v>
@@ -8908,10 +8908,10 @@
         <v>704</v>
       </c>
       <c r="H172">
-        <v>453411</v>
+        <v>453603</v>
       </c>
       <c r="I172">
-        <v>124938</v>
+        <v>125010</v>
       </c>
       <c r="J172" t="s">
         <v>719</v>
@@ -8943,10 +8943,10 @@
         <v>704</v>
       </c>
       <c r="H173">
-        <v>86903</v>
+        <v>86957</v>
       </c>
       <c r="I173">
-        <v>53060</v>
+        <v>53097</v>
       </c>
       <c r="J173" t="s">
         <v>717</v>
@@ -8978,10 +8978,10 @@
         <v>704</v>
       </c>
       <c r="H174">
-        <v>311200</v>
+        <v>311308</v>
       </c>
       <c r="I174">
-        <v>67992</v>
+        <v>68016</v>
       </c>
       <c r="J174" t="s">
         <v>710</v>
@@ -9013,10 +9013,10 @@
         <v>704</v>
       </c>
       <c r="H175">
-        <v>125701</v>
+        <v>125775</v>
       </c>
       <c r="I175">
-        <v>69063</v>
+        <v>69114</v>
       </c>
       <c r="J175" t="s">
         <v>766</v>
@@ -9048,10 +9048,10 @@
         <v>704</v>
       </c>
       <c r="H176">
-        <v>161779</v>
+        <v>161981</v>
       </c>
       <c r="I176">
-        <v>77616</v>
+        <v>77718</v>
       </c>
       <c r="J176" t="s">
         <v>717</v>
@@ -9083,10 +9083,10 @@
         <v>705</v>
       </c>
       <c r="H177">
-        <v>70525</v>
+        <v>70556</v>
       </c>
       <c r="I177">
-        <v>15223</v>
+        <v>15238</v>
       </c>
       <c r="J177" t="s">
         <v>767</v>
@@ -9118,10 +9118,10 @@
         <v>704</v>
       </c>
       <c r="H178">
-        <v>71327</v>
+        <v>71365</v>
       </c>
       <c r="I178">
-        <v>48908</v>
+        <v>48940</v>
       </c>
       <c r="J178" t="s">
         <v>717</v>
@@ -9153,10 +9153,10 @@
         <v>706</v>
       </c>
       <c r="H179">
-        <v>425132</v>
+        <v>425225</v>
       </c>
       <c r="I179">
-        <v>27003</v>
+        <v>27009</v>
       </c>
       <c r="J179" t="s">
         <v>768</v>
@@ -9188,10 +9188,10 @@
         <v>704</v>
       </c>
       <c r="H180">
-        <v>66896</v>
+        <v>66927</v>
       </c>
       <c r="I180">
-        <v>31286</v>
+        <v>31302</v>
       </c>
       <c r="J180" t="s">
         <v>717</v>
@@ -9223,10 +9223,10 @@
         <v>704</v>
       </c>
       <c r="H181">
-        <v>89117</v>
+        <v>89165</v>
       </c>
       <c r="I181">
-        <v>51943</v>
+        <v>51979</v>
       </c>
       <c r="J181" t="s">
         <v>769</v>
@@ -9258,10 +9258,10 @@
         <v>704</v>
       </c>
       <c r="H182">
-        <v>317727</v>
+        <v>317791</v>
       </c>
       <c r="I182">
-        <v>54133</v>
+        <v>54150</v>
       </c>
       <c r="J182" t="s">
         <v>770</v>
@@ -9293,10 +9293,10 @@
         <v>704</v>
       </c>
       <c r="H183">
-        <v>191091</v>
+        <v>191194</v>
       </c>
       <c r="I183">
-        <v>87537</v>
+        <v>87610</v>
       </c>
       <c r="J183" t="s">
         <v>717</v>
@@ -9328,10 +9328,10 @@
         <v>704</v>
       </c>
       <c r="H184">
-        <v>1604709</v>
+        <v>1604989</v>
       </c>
       <c r="I184">
-        <v>78955</v>
+        <v>78971</v>
       </c>
       <c r="J184" t="s">
         <v>717</v>
@@ -9363,10 +9363,10 @@
         <v>704</v>
       </c>
       <c r="H185">
-        <v>225759</v>
+        <v>225782</v>
       </c>
       <c r="I185">
-        <v>45343</v>
+        <v>45355</v>
       </c>
       <c r="J185" t="s">
         <v>735</v>
@@ -9398,10 +9398,10 @@
         <v>704</v>
       </c>
       <c r="H186">
-        <v>245723</v>
+        <v>245832</v>
       </c>
       <c r="I186">
-        <v>125352</v>
+        <v>125414</v>
       </c>
       <c r="J186" t="s">
         <v>771</v>
@@ -9433,10 +9433,10 @@
         <v>704</v>
       </c>
       <c r="H187">
-        <v>134493</v>
+        <v>134603</v>
       </c>
       <c r="I187">
-        <v>54782</v>
+        <v>54814</v>
       </c>
       <c r="J187" t="s">
         <v>729</v>
@@ -9468,10 +9468,10 @@
         <v>704</v>
       </c>
       <c r="H188">
-        <v>66773</v>
+        <v>66819</v>
       </c>
       <c r="I188">
-        <v>40788</v>
+        <v>40815</v>
       </c>
       <c r="J188" t="s">
         <v>737</v>
@@ -9503,10 +9503,10 @@
         <v>704</v>
       </c>
       <c r="H189">
-        <v>172004</v>
+        <v>172122</v>
       </c>
       <c r="I189">
-        <v>112588</v>
+        <v>112667</v>
       </c>
       <c r="J189" t="s">
         <v>719</v>
@@ -9538,10 +9538,10 @@
         <v>704</v>
       </c>
       <c r="H190">
-        <v>92633</v>
+        <v>92686</v>
       </c>
       <c r="I190">
-        <v>55609</v>
+        <v>55648</v>
       </c>
       <c r="J190" t="s">
         <v>772</v>
@@ -9573,10 +9573,10 @@
         <v>704</v>
       </c>
       <c r="H191">
-        <v>221870</v>
+        <v>221961</v>
       </c>
       <c r="I191">
-        <v>105154</v>
+        <v>105206</v>
       </c>
       <c r="J191" t="s">
         <v>720</v>
@@ -9608,10 +9608,10 @@
         <v>704</v>
       </c>
       <c r="H192">
-        <v>119185</v>
+        <v>119250</v>
       </c>
       <c r="I192">
-        <v>55347</v>
+        <v>55395</v>
       </c>
       <c r="J192" t="s">
         <v>717</v>
@@ -9643,10 +9643,10 @@
         <v>704</v>
       </c>
       <c r="H193">
-        <v>72770</v>
+        <v>72818</v>
       </c>
       <c r="I193">
-        <v>53246</v>
+        <v>53286</v>
       </c>
       <c r="J193" t="s">
         <v>717</v>
@@ -9678,10 +9678,10 @@
         <v>704</v>
       </c>
       <c r="H194">
-        <v>160882</v>
+        <v>160914</v>
       </c>
       <c r="I194">
-        <v>45837</v>
+        <v>45848</v>
       </c>
       <c r="J194" t="s">
         <v>766</v>
@@ -9713,10 +9713,10 @@
         <v>704</v>
       </c>
       <c r="H195">
-        <v>104990</v>
+        <v>105062</v>
       </c>
       <c r="I195">
-        <v>41951</v>
+        <v>41960</v>
       </c>
       <c r="J195" t="s">
         <v>717</v>
@@ -9748,10 +9748,10 @@
         <v>704</v>
       </c>
       <c r="H196">
-        <v>76718</v>
+        <v>76763</v>
       </c>
       <c r="I196">
-        <v>40154</v>
+        <v>40181</v>
       </c>
       <c r="J196" t="s">
         <v>717</v>
@@ -9783,10 +9783,10 @@
         <v>704</v>
       </c>
       <c r="H197">
-        <v>276493</v>
+        <v>276547</v>
       </c>
       <c r="I197">
-        <v>68730</v>
+        <v>68748</v>
       </c>
       <c r="J197" t="s">
         <v>739</v>
@@ -9818,10 +9818,10 @@
         <v>704</v>
       </c>
       <c r="H198">
-        <v>120026</v>
+        <v>120064</v>
       </c>
       <c r="I198">
-        <v>54801</v>
+        <v>54826</v>
       </c>
       <c r="J198" t="s">
         <v>740</v>
@@ -9853,10 +9853,10 @@
         <v>704</v>
       </c>
       <c r="H199">
-        <v>111698</v>
+        <v>111766</v>
       </c>
       <c r="I199">
-        <v>60652</v>
+        <v>60696</v>
       </c>
       <c r="J199" t="s">
         <v>729</v>
@@ -9888,10 +9888,10 @@
         <v>704</v>
       </c>
       <c r="H200">
-        <v>112562</v>
+        <v>112608</v>
       </c>
       <c r="I200">
-        <v>40675</v>
+        <v>40694</v>
       </c>
       <c r="J200" t="s">
         <v>770</v>
@@ -9923,10 +9923,10 @@
         <v>704</v>
       </c>
       <c r="H201">
-        <v>128823</v>
+        <v>128885</v>
       </c>
       <c r="I201">
-        <v>47386</v>
+        <v>47414</v>
       </c>
       <c r="J201" t="s">
         <v>717</v>
@@ -9958,10 +9958,10 @@
         <v>704</v>
       </c>
       <c r="H202">
-        <v>146105</v>
+        <v>146210</v>
       </c>
       <c r="I202">
-        <v>71456</v>
+        <v>71524</v>
       </c>
       <c r="J202" t="s">
         <v>727</v>
@@ -9993,10 +9993,10 @@
         <v>704</v>
       </c>
       <c r="H203">
-        <v>104723</v>
+        <v>104742</v>
       </c>
       <c r="I203">
-        <v>46593</v>
+        <v>46606</v>
       </c>
       <c r="J203" t="s">
         <v>719</v>
@@ -10028,10 +10028,10 @@
         <v>704</v>
       </c>
       <c r="H204">
-        <v>261978</v>
+        <v>262067</v>
       </c>
       <c r="I204">
-        <v>65973</v>
+        <v>65996</v>
       </c>
       <c r="J204" t="s">
         <v>740</v>
@@ -10063,10 +10063,10 @@
         <v>704</v>
       </c>
       <c r="H205">
-        <v>325112</v>
+        <v>325252</v>
       </c>
       <c r="I205">
-        <v>101962</v>
+        <v>102015</v>
       </c>
       <c r="J205" t="s">
         <v>719</v>
@@ -10098,10 +10098,10 @@
         <v>704</v>
       </c>
       <c r="H206">
-        <v>119570</v>
+        <v>119629</v>
       </c>
       <c r="I206">
-        <v>59846</v>
+        <v>59880</v>
       </c>
       <c r="J206" t="s">
         <v>770</v>
@@ -10133,10 +10133,10 @@
         <v>704</v>
       </c>
       <c r="H207">
-        <v>155652</v>
+        <v>155705</v>
       </c>
       <c r="I207">
-        <v>76008</v>
+        <v>76045</v>
       </c>
       <c r="J207" t="s">
         <v>729</v>
@@ -10168,10 +10168,10 @@
         <v>704</v>
       </c>
       <c r="H208">
-        <v>228065</v>
+        <v>228091</v>
       </c>
       <c r="I208">
-        <v>36045</v>
+        <v>36052</v>
       </c>
       <c r="J208" t="s">
         <v>735</v>
@@ -10203,10 +10203,10 @@
         <v>704</v>
       </c>
       <c r="H209">
-        <v>714180</v>
+        <v>714536</v>
       </c>
       <c r="I209">
-        <v>87568</v>
+        <v>87613</v>
       </c>
       <c r="J209" t="s">
         <v>773</v>
@@ -10238,10 +10238,10 @@
         <v>704</v>
       </c>
       <c r="H210">
-        <v>190429</v>
+        <v>190493</v>
       </c>
       <c r="I210">
-        <v>95640</v>
+        <v>95682</v>
       </c>
       <c r="J210" t="s">
         <v>717</v>
@@ -10273,10 +10273,10 @@
         <v>704</v>
       </c>
       <c r="H211">
-        <v>337369</v>
+        <v>337517</v>
       </c>
       <c r="I211">
-        <v>146646</v>
+        <v>146733</v>
       </c>
       <c r="J211" t="s">
         <v>717</v>
@@ -10308,10 +10308,10 @@
         <v>704</v>
       </c>
       <c r="H212">
-        <v>396789</v>
+        <v>396925</v>
       </c>
       <c r="I212">
-        <v>204695</v>
+        <v>204788</v>
       </c>
       <c r="J212" t="s">
         <v>719</v>
@@ -10343,10 +10343,10 @@
         <v>704</v>
       </c>
       <c r="H213">
-        <v>181433</v>
+        <v>181531</v>
       </c>
       <c r="I213">
-        <v>75528</v>
+        <v>75579</v>
       </c>
       <c r="J213" t="s">
         <v>737</v>
@@ -10378,10 +10378,10 @@
         <v>704</v>
       </c>
       <c r="H214">
-        <v>140428</v>
+        <v>140523</v>
       </c>
       <c r="I214">
-        <v>74383</v>
+        <v>74454</v>
       </c>
       <c r="J214" t="s">
         <v>720</v>
@@ -10413,10 +10413,10 @@
         <v>704</v>
       </c>
       <c r="H215">
-        <v>201547</v>
+        <v>201691</v>
       </c>
       <c r="I215">
-        <v>77556</v>
+        <v>77621</v>
       </c>
       <c r="J215" t="s">
         <v>717</v>
@@ -10448,10 +10448,10 @@
         <v>704</v>
       </c>
       <c r="H216">
-        <v>144912</v>
+        <v>144991</v>
       </c>
       <c r="I216">
-        <v>89242</v>
+        <v>89313</v>
       </c>
       <c r="J216" t="s">
         <v>729</v>
@@ -10483,10 +10483,10 @@
         <v>704</v>
       </c>
       <c r="H217">
-        <v>338201</v>
+        <v>338361</v>
       </c>
       <c r="I217">
-        <v>111231</v>
+        <v>111267</v>
       </c>
       <c r="J217" t="s">
         <v>717</v>
@@ -10518,10 +10518,10 @@
         <v>704</v>
       </c>
       <c r="H218">
-        <v>477728</v>
+        <v>477953</v>
       </c>
       <c r="I218">
-        <v>200860</v>
+        <v>200951</v>
       </c>
       <c r="J218" t="s">
         <v>717</v>
@@ -10553,10 +10553,10 @@
         <v>704</v>
       </c>
       <c r="H219">
-        <v>282412</v>
+        <v>282469</v>
       </c>
       <c r="I219">
-        <v>119604</v>
+        <v>119640</v>
       </c>
       <c r="J219" t="s">
         <v>774</v>
@@ -10588,10 +10588,10 @@
         <v>704</v>
       </c>
       <c r="H220">
-        <v>147991</v>
+        <v>148094</v>
       </c>
       <c r="I220">
-        <v>65267</v>
+        <v>65313</v>
       </c>
       <c r="J220" t="s">
         <v>735</v>
@@ -10623,10 +10623,10 @@
         <v>704</v>
       </c>
       <c r="H221">
-        <v>168421</v>
+        <v>168550</v>
       </c>
       <c r="I221">
-        <v>62957</v>
+        <v>62998</v>
       </c>
       <c r="J221" t="s">
         <v>729</v>
@@ -10658,10 +10658,10 @@
         <v>704</v>
       </c>
       <c r="H222">
-        <v>151593</v>
+        <v>151655</v>
       </c>
       <c r="I222">
-        <v>76111</v>
+        <v>76156</v>
       </c>
       <c r="J222" t="s">
         <v>717</v>
@@ -10693,10 +10693,10 @@
         <v>704</v>
       </c>
       <c r="H223">
-        <v>360774</v>
+        <v>360896</v>
       </c>
       <c r="I223">
-        <v>52256</v>
+        <v>52290</v>
       </c>
       <c r="J223" t="s">
         <v>717</v>
@@ -10728,10 +10728,10 @@
         <v>704</v>
       </c>
       <c r="H224">
-        <v>148369</v>
+        <v>148480</v>
       </c>
       <c r="I224">
-        <v>92355</v>
+        <v>92428</v>
       </c>
       <c r="J224" t="s">
         <v>717</v>
@@ -10763,10 +10763,10 @@
         <v>704</v>
       </c>
       <c r="H225">
-        <v>239944</v>
+        <v>240121</v>
       </c>
       <c r="I225">
-        <v>80756</v>
+        <v>80818</v>
       </c>
       <c r="J225" t="s">
         <v>720</v>
@@ -10798,10 +10798,10 @@
         <v>704</v>
       </c>
       <c r="H226">
-        <v>384023</v>
+        <v>384178</v>
       </c>
       <c r="I226">
-        <v>186217</v>
+        <v>186307</v>
       </c>
       <c r="J226" t="s">
         <v>729</v>
@@ -10833,10 +10833,10 @@
         <v>704</v>
       </c>
       <c r="H227">
-        <v>683827</v>
+        <v>684005</v>
       </c>
       <c r="I227">
-        <v>133519</v>
+        <v>133555</v>
       </c>
       <c r="J227" t="s">
         <v>763</v>
@@ -10868,10 +10868,10 @@
         <v>704</v>
       </c>
       <c r="H228">
-        <v>179949</v>
+        <v>180101</v>
       </c>
       <c r="I228">
-        <v>112184</v>
+        <v>112281</v>
       </c>
       <c r="J228" t="s">
         <v>717</v>
@@ -10903,10 +10903,10 @@
         <v>704</v>
       </c>
       <c r="H229">
-        <v>165370</v>
+        <v>165524</v>
       </c>
       <c r="I229">
-        <v>86026</v>
+        <v>86113</v>
       </c>
       <c r="J229" t="s">
         <v>735</v>
@@ -10938,10 +10938,10 @@
         <v>704</v>
       </c>
       <c r="H230">
-        <v>175266</v>
+        <v>175380</v>
       </c>
       <c r="I230">
-        <v>75302</v>
+        <v>75356</v>
       </c>
       <c r="J230" t="s">
         <v>717</v>
@@ -10973,10 +10973,10 @@
         <v>704</v>
       </c>
       <c r="H231">
-        <v>406036</v>
+        <v>406111</v>
       </c>
       <c r="I231">
-        <v>122603</v>
+        <v>122633</v>
       </c>
       <c r="J231" t="s">
         <v>737</v>
@@ -11008,10 +11008,10 @@
         <v>704</v>
       </c>
       <c r="H232">
-        <v>315100</v>
+        <v>315263</v>
       </c>
       <c r="I232">
-        <v>156614</v>
+        <v>156700</v>
       </c>
       <c r="J232" t="s">
         <v>721</v>
@@ -11043,10 +11043,10 @@
         <v>704</v>
       </c>
       <c r="H233">
-        <v>642099</v>
+        <v>642272</v>
       </c>
       <c r="I233">
-        <v>197765</v>
+        <v>197840</v>
       </c>
       <c r="J233" t="s">
         <v>721</v>
@@ -11078,10 +11078,10 @@
         <v>704</v>
       </c>
       <c r="H234">
-        <v>211454</v>
+        <v>211612</v>
       </c>
       <c r="I234">
-        <v>79528</v>
+        <v>79580</v>
       </c>
       <c r="J234" t="s">
         <v>740</v>
@@ -11113,10 +11113,10 @@
         <v>704</v>
       </c>
       <c r="H235">
-        <v>679659</v>
+        <v>679791</v>
       </c>
       <c r="I235">
-        <v>118533</v>
+        <v>118565</v>
       </c>
       <c r="J235" t="s">
         <v>710</v>
@@ -11148,10 +11148,10 @@
         <v>704</v>
       </c>
       <c r="H236">
-        <v>649499</v>
+        <v>649645</v>
       </c>
       <c r="I236">
-        <v>145114</v>
+        <v>145162</v>
       </c>
       <c r="J236" t="s">
         <v>719</v>
@@ -11183,10 +11183,10 @@
         <v>704</v>
       </c>
       <c r="H237">
-        <v>341446</v>
+        <v>341637</v>
       </c>
       <c r="I237">
-        <v>83444</v>
+        <v>83485</v>
       </c>
       <c r="J237" t="s">
         <v>719</v>
@@ -11218,10 +11218,10 @@
         <v>704</v>
       </c>
       <c r="H238">
-        <v>471411</v>
+        <v>471498</v>
       </c>
       <c r="I238">
-        <v>96117</v>
+        <v>96146</v>
       </c>
       <c r="J238" t="s">
         <v>775</v>
@@ -11253,10 +11253,10 @@
         <v>704</v>
       </c>
       <c r="H239">
-        <v>437665</v>
+        <v>437836</v>
       </c>
       <c r="I239">
-        <v>193275</v>
+        <v>193375</v>
       </c>
       <c r="J239" t="s">
         <v>735</v>
@@ -11288,10 +11288,10 @@
         <v>704</v>
       </c>
       <c r="H240">
-        <v>225975</v>
+        <v>226064</v>
       </c>
       <c r="I240">
-        <v>95870</v>
+        <v>95917</v>
       </c>
       <c r="J240" t="s">
         <v>735</v>
@@ -11323,10 +11323,10 @@
         <v>704</v>
       </c>
       <c r="H241">
-        <v>430114</v>
+        <v>430238</v>
       </c>
       <c r="I241">
-        <v>153318</v>
+        <v>153384</v>
       </c>
       <c r="J241" t="s">
         <v>735</v>
@@ -11358,10 +11358,10 @@
         <v>704</v>
       </c>
       <c r="H242">
-        <v>739521</v>
+        <v>739751</v>
       </c>
       <c r="I242">
-        <v>290574</v>
+        <v>290668</v>
       </c>
       <c r="J242" t="s">
         <v>719</v>
@@ -11393,10 +11393,10 @@
         <v>704</v>
       </c>
       <c r="H243">
-        <v>345834</v>
+        <v>345924</v>
       </c>
       <c r="I243">
-        <v>119752</v>
+        <v>119791</v>
       </c>
       <c r="J243" t="s">
         <v>717</v>
@@ -11428,10 +11428,10 @@
         <v>704</v>
       </c>
       <c r="H244">
-        <v>333614</v>
+        <v>333749</v>
       </c>
       <c r="I244">
-        <v>107131</v>
+        <v>107177</v>
       </c>
       <c r="J244" t="s">
         <v>735</v>
@@ -11463,10 +11463,10 @@
         <v>704</v>
       </c>
       <c r="H245">
-        <v>432809</v>
+        <v>432931</v>
       </c>
       <c r="I245">
-        <v>148923</v>
+        <v>148993</v>
       </c>
       <c r="J245" t="s">
         <v>735</v>
@@ -11498,10 +11498,10 @@
         <v>704</v>
       </c>
       <c r="H246">
-        <v>561584</v>
+        <v>561764</v>
       </c>
       <c r="I246">
-        <v>176614</v>
+        <v>176688</v>
       </c>
       <c r="J246" t="s">
         <v>719</v>
@@ -11533,10 +11533,10 @@
         <v>704</v>
       </c>
       <c r="H247">
-        <v>622918</v>
+        <v>623106</v>
       </c>
       <c r="I247">
-        <v>174834</v>
+        <v>174882</v>
       </c>
       <c r="J247" t="s">
         <v>719</v>
@@ -11568,10 +11568,10 @@
         <v>704</v>
       </c>
       <c r="H248">
-        <v>420488</v>
+        <v>420610</v>
       </c>
       <c r="I248">
-        <v>226617</v>
+        <v>226710</v>
       </c>
       <c r="J248" t="s">
         <v>717</v>
@@ -11603,10 +11603,10 @@
         <v>704</v>
       </c>
       <c r="H249">
-        <v>404386</v>
+        <v>404549</v>
       </c>
       <c r="I249">
-        <v>179884</v>
+        <v>179968</v>
       </c>
       <c r="J249" t="s">
         <v>719</v>
@@ -11638,10 +11638,10 @@
         <v>704</v>
       </c>
       <c r="H250">
-        <v>417568</v>
+        <v>417615</v>
       </c>
       <c r="I250">
-        <v>120867</v>
+        <v>120890</v>
       </c>
       <c r="J250" t="s">
         <v>719</v>
@@ -11673,10 +11673,10 @@
         <v>704</v>
       </c>
       <c r="H251">
-        <v>403022</v>
+        <v>403087</v>
       </c>
       <c r="I251">
-        <v>161542</v>
+        <v>161578</v>
       </c>
       <c r="J251" t="s">
         <v>719</v>
@@ -11708,10 +11708,10 @@
         <v>704</v>
       </c>
       <c r="H252">
-        <v>27729</v>
+        <v>27743</v>
       </c>
       <c r="I252">
-        <v>10594</v>
+        <v>10600</v>
       </c>
       <c r="J252" t="s">
         <v>776</v>
@@ -11743,10 +11743,10 @@
         <v>704</v>
       </c>
       <c r="H253">
-        <v>563653</v>
+        <v>563815</v>
       </c>
       <c r="I253">
-        <v>196843</v>
+        <v>196901</v>
       </c>
       <c r="J253" t="s">
         <v>729</v>
@@ -11813,10 +11813,10 @@
         <v>704</v>
       </c>
       <c r="H255">
-        <v>625559</v>
+        <v>625706</v>
       </c>
       <c r="I255">
-        <v>143027</v>
+        <v>143063</v>
       </c>
       <c r="J255" t="s">
         <v>735</v>
@@ -11848,10 +11848,10 @@
         <v>704</v>
       </c>
       <c r="H256">
-        <v>708320</v>
+        <v>708439</v>
       </c>
       <c r="I256">
-        <v>192583</v>
+        <v>192639</v>
       </c>
       <c r="J256" t="s">
         <v>717</v>
@@ -11883,10 +11883,10 @@
         <v>704</v>
       </c>
       <c r="H257">
-        <v>374422</v>
+        <v>374613</v>
       </c>
       <c r="I257">
-        <v>216927</v>
+        <v>217045</v>
       </c>
       <c r="J257" t="s">
         <v>719</v>
@@ -11918,10 +11918,10 @@
         <v>704</v>
       </c>
       <c r="H258">
-        <v>373826</v>
+        <v>373994</v>
       </c>
       <c r="I258">
-        <v>158558</v>
+        <v>158644</v>
       </c>
       <c r="J258" t="s">
         <v>777</v>
@@ -11953,10 +11953,10 @@
         <v>704</v>
       </c>
       <c r="H259">
-        <v>641625</v>
+        <v>641774</v>
       </c>
       <c r="I259">
-        <v>147560</v>
+        <v>147607</v>
       </c>
       <c r="J259" t="s">
         <v>723</v>
@@ -11988,10 +11988,10 @@
         <v>704</v>
       </c>
       <c r="H260">
-        <v>583205</v>
+        <v>583374</v>
       </c>
       <c r="I260">
-        <v>176761</v>
+        <v>176818</v>
       </c>
       <c r="J260" t="s">
         <v>717</v>
@@ -12023,10 +12023,10 @@
         <v>704</v>
       </c>
       <c r="H261">
-        <v>652849</v>
+        <v>653180</v>
       </c>
       <c r="I261">
-        <v>218838</v>
+        <v>218949</v>
       </c>
       <c r="J261" t="s">
         <v>737</v>
@@ -12058,10 +12058,10 @@
         <v>704</v>
       </c>
       <c r="H262">
-        <v>622016</v>
+        <v>622276</v>
       </c>
       <c r="I262">
-        <v>302337</v>
+        <v>302469</v>
       </c>
       <c r="J262" t="s">
         <v>737</v>
@@ -12093,10 +12093,10 @@
         <v>704</v>
       </c>
       <c r="H263">
-        <v>373713</v>
+        <v>373883</v>
       </c>
       <c r="I263">
-        <v>205498</v>
+        <v>205598</v>
       </c>
       <c r="J263" t="s">
         <v>717</v>
@@ -12128,10 +12128,10 @@
         <v>702</v>
       </c>
       <c r="H264">
-        <v>219759</v>
+        <v>219801</v>
       </c>
       <c r="I264">
-        <v>39867</v>
+        <v>39882</v>
       </c>
       <c r="J264" t="s">
         <v>711</v>
@@ -12163,10 +12163,10 @@
         <v>702</v>
       </c>
       <c r="H265">
-        <v>322008</v>
+        <v>322049</v>
       </c>
       <c r="I265">
-        <v>41159</v>
+        <v>41172</v>
       </c>
       <c r="J265" t="s">
         <v>778</v>
@@ -12198,10 +12198,10 @@
         <v>702</v>
       </c>
       <c r="H266">
-        <v>501027</v>
+        <v>501200</v>
       </c>
       <c r="I266">
-        <v>29567</v>
+        <v>29574</v>
       </c>
       <c r="J266" t="s">
         <v>779</v>
@@ -12233,10 +12233,10 @@
         <v>702</v>
       </c>
       <c r="H267">
-        <v>405884</v>
+        <v>405995</v>
       </c>
       <c r="I267">
-        <v>54530</v>
+        <v>54551</v>
       </c>
       <c r="J267" t="s">
         <v>780</v>
@@ -12303,10 +12303,10 @@
         <v>702</v>
       </c>
       <c r="H269">
-        <v>312627</v>
+        <v>312641</v>
       </c>
       <c r="I269">
-        <v>41678</v>
+        <v>41686</v>
       </c>
       <c r="J269" t="s">
         <v>711</v>
@@ -12338,10 +12338,10 @@
         <v>702</v>
       </c>
       <c r="H270">
-        <v>292444</v>
+        <v>292463</v>
       </c>
       <c r="I270">
-        <v>46327</v>
+        <v>46334</v>
       </c>
       <c r="J270" t="s">
         <v>782</v>
@@ -12373,10 +12373,10 @@
         <v>704</v>
       </c>
       <c r="H271">
-        <v>184941</v>
+        <v>184998</v>
       </c>
       <c r="I271">
-        <v>49855</v>
+        <v>49874</v>
       </c>
       <c r="J271" t="s">
         <v>783</v>
@@ -12408,10 +12408,10 @@
         <v>702</v>
       </c>
       <c r="H272">
-        <v>185870</v>
+        <v>185925</v>
       </c>
       <c r="I272">
-        <v>51039</v>
+        <v>51061</v>
       </c>
       <c r="J272" t="s">
         <v>711</v>
@@ -12443,10 +12443,10 @@
         <v>704</v>
       </c>
       <c r="H273">
-        <v>389627</v>
+        <v>389719</v>
       </c>
       <c r="I273">
-        <v>52958</v>
+        <v>52980</v>
       </c>
       <c r="J273" t="s">
         <v>784</v>
@@ -12478,10 +12478,10 @@
         <v>704</v>
       </c>
       <c r="H274">
-        <v>225578</v>
+        <v>225635</v>
       </c>
       <c r="I274">
-        <v>59265</v>
+        <v>59288</v>
       </c>
       <c r="J274" t="s">
         <v>785</v>
@@ -12513,10 +12513,10 @@
         <v>702</v>
       </c>
       <c r="H275">
-        <v>235012</v>
+        <v>235128</v>
       </c>
       <c r="I275">
-        <v>61544</v>
+        <v>61592</v>
       </c>
       <c r="J275" t="s">
         <v>782</v>
@@ -12548,10 +12548,10 @@
         <v>704</v>
       </c>
       <c r="H276">
-        <v>325813</v>
+        <v>325911</v>
       </c>
       <c r="I276">
-        <v>65597</v>
+        <v>65619</v>
       </c>
       <c r="J276" t="s">
         <v>786</v>
@@ -12583,10 +12583,10 @@
         <v>702</v>
       </c>
       <c r="H277">
-        <v>342480</v>
+        <v>342637</v>
       </c>
       <c r="I277">
-        <v>89046</v>
+        <v>89071</v>
       </c>
       <c r="J277" t="s">
         <v>711</v>
@@ -12618,10 +12618,10 @@
         <v>702</v>
       </c>
       <c r="H278">
-        <v>542882</v>
+        <v>543000</v>
       </c>
       <c r="I278">
-        <v>90423</v>
+        <v>90448</v>
       </c>
       <c r="J278" t="s">
         <v>711</v>
@@ -12653,10 +12653,10 @@
         <v>702</v>
       </c>
       <c r="H279">
-        <v>487853</v>
+        <v>487990</v>
       </c>
       <c r="I279">
-        <v>117217</v>
+        <v>117275</v>
       </c>
       <c r="J279" t="s">
         <v>787</v>
@@ -12688,10 +12688,10 @@
         <v>702</v>
       </c>
       <c r="H280">
-        <v>643877</v>
+        <v>644086</v>
       </c>
       <c r="I280">
-        <v>117277</v>
+        <v>117317</v>
       </c>
       <c r="J280" t="s">
         <v>788</v>
@@ -12723,10 +12723,10 @@
         <v>702</v>
       </c>
       <c r="H281">
-        <v>50689</v>
+        <v>50696</v>
       </c>
       <c r="I281">
-        <v>15200</v>
+        <v>15203</v>
       </c>
       <c r="J281" t="s">
         <v>711</v>
@@ -12758,10 +12758,10 @@
         <v>704</v>
       </c>
       <c r="H282">
-        <v>684470</v>
+        <v>684603</v>
       </c>
       <c r="I282">
-        <v>165583</v>
+        <v>165630</v>
       </c>
       <c r="J282" t="s">
         <v>719</v>
@@ -12793,10 +12793,10 @@
         <v>702</v>
       </c>
       <c r="H283">
-        <v>437183</v>
+        <v>437286</v>
       </c>
       <c r="I283">
-        <v>177831</v>
+        <v>177869</v>
       </c>
       <c r="J283" t="s">
         <v>789</v>
@@ -12828,10 +12828,10 @@
         <v>702</v>
       </c>
       <c r="H284">
-        <v>709972</v>
+        <v>710164</v>
       </c>
       <c r="I284">
-        <v>194557</v>
+        <v>194624</v>
       </c>
       <c r="J284" t="s">
         <v>782</v>
@@ -12863,10 +12863,10 @@
         <v>702</v>
       </c>
       <c r="H285">
-        <v>795220</v>
+        <v>795545</v>
       </c>
       <c r="I285">
-        <v>200104</v>
+        <v>200234</v>
       </c>
       <c r="J285" t="s">
         <v>790</v>
@@ -12898,10 +12898,10 @@
         <v>704</v>
       </c>
       <c r="H286">
-        <v>641762</v>
+        <v>641932</v>
       </c>
       <c r="I286">
-        <v>218426</v>
+        <v>218501</v>
       </c>
       <c r="J286" t="s">
         <v>717</v>
@@ -12933,10 +12933,10 @@
         <v>704</v>
       </c>
       <c r="H287">
-        <v>735786</v>
+        <v>735980</v>
       </c>
       <c r="I287">
-        <v>237713</v>
+        <v>237792</v>
       </c>
       <c r="J287" t="s">
         <v>719</v>
@@ -12968,10 +12968,10 @@
         <v>702</v>
       </c>
       <c r="H288">
-        <v>899446</v>
+        <v>899654</v>
       </c>
       <c r="I288">
-        <v>301303</v>
+        <v>301386</v>
       </c>
       <c r="J288" t="s">
         <v>790</v>
@@ -13003,10 +13003,10 @@
         <v>704</v>
       </c>
       <c r="H289">
-        <v>23027</v>
+        <v>23029</v>
       </c>
       <c r="I289">
-        <v>2219</v>
+        <v>2220</v>
       </c>
       <c r="J289" t="s">
         <v>791</v>
@@ -13073,10 +13073,10 @@
         <v>704</v>
       </c>
       <c r="H291">
-        <v>28103</v>
+        <v>28104</v>
       </c>
       <c r="I291">
-        <v>3650</v>
+        <v>3651</v>
       </c>
       <c r="J291" t="s">
         <v>792</v>
@@ -13108,10 +13108,10 @@
         <v>704</v>
       </c>
       <c r="H292">
-        <v>27394</v>
+        <v>27402</v>
       </c>
       <c r="I292">
-        <v>6088</v>
+        <v>6090</v>
       </c>
       <c r="J292" t="s">
         <v>792</v>
@@ -13143,7 +13143,7 @@
         <v>705</v>
       </c>
       <c r="H293">
-        <v>30021</v>
+        <v>30036</v>
       </c>
       <c r="I293">
         <v>2218</v>
@@ -13178,10 +13178,10 @@
         <v>704</v>
       </c>
       <c r="H294">
-        <v>13106</v>
+        <v>13116</v>
       </c>
       <c r="I294">
-        <v>2692</v>
+        <v>2693</v>
       </c>
       <c r="J294" t="s">
         <v>748</v>
@@ -13248,7 +13248,7 @@
         <v>704</v>
       </c>
       <c r="H296">
-        <v>44365</v>
+        <v>44367</v>
       </c>
       <c r="I296">
         <v>2899</v>
@@ -13283,10 +13283,10 @@
         <v>704</v>
       </c>
       <c r="H297">
-        <v>10900</v>
+        <v>10902</v>
       </c>
       <c r="I297">
-        <v>3823</v>
+        <v>3824</v>
       </c>
       <c r="J297" t="s">
         <v>745</v>
@@ -13353,10 +13353,10 @@
         <v>704</v>
       </c>
       <c r="H299">
-        <v>32248</v>
+        <v>32250</v>
       </c>
       <c r="I299">
-        <v>7133</v>
+        <v>7134</v>
       </c>
       <c r="J299" t="s">
         <v>794</v>
@@ -13388,7 +13388,7 @@
         <v>704</v>
       </c>
       <c r="H300">
-        <v>27382</v>
+        <v>27387</v>
       </c>
       <c r="I300">
         <v>7152</v>
@@ -13423,10 +13423,10 @@
         <v>704</v>
       </c>
       <c r="H301">
-        <v>35826</v>
+        <v>35830</v>
       </c>
       <c r="I301">
-        <v>8848</v>
+        <v>8849</v>
       </c>
       <c r="J301" t="s">
         <v>747</v>
@@ -13493,10 +13493,10 @@
         <v>704</v>
       </c>
       <c r="H303">
-        <v>51623</v>
+        <v>51643</v>
       </c>
       <c r="I303">
-        <v>10021</v>
+        <v>10022</v>
       </c>
       <c r="J303" t="s">
         <v>745</v>
@@ -13528,10 +13528,10 @@
         <v>704</v>
       </c>
       <c r="H304">
-        <v>3654</v>
+        <v>3660</v>
       </c>
       <c r="I304">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="J304" t="s">
         <v>794</v>
@@ -13598,10 +13598,10 @@
         <v>704</v>
       </c>
       <c r="H306">
-        <v>43573</v>
+        <v>43602</v>
       </c>
       <c r="I306">
-        <v>10602</v>
+        <v>10603</v>
       </c>
       <c r="J306" t="s">
         <v>794</v>
@@ -13633,10 +13633,10 @@
         <v>704</v>
       </c>
       <c r="H307">
-        <v>56508</v>
+        <v>56522</v>
       </c>
       <c r="I307">
-        <v>10627</v>
+        <v>10631</v>
       </c>
       <c r="J307" t="s">
         <v>745</v>
@@ -13668,10 +13668,10 @@
         <v>704</v>
       </c>
       <c r="H308">
-        <v>62851</v>
+        <v>62882</v>
       </c>
       <c r="I308">
-        <v>10855</v>
+        <v>10858</v>
       </c>
       <c r="J308" t="s">
         <v>745</v>
@@ -13703,10 +13703,10 @@
         <v>704</v>
       </c>
       <c r="H309">
-        <v>37356</v>
+        <v>37357</v>
       </c>
       <c r="I309">
-        <v>15236</v>
+        <v>15237</v>
       </c>
       <c r="J309" t="s">
         <v>745</v>
@@ -13738,10 +13738,10 @@
         <v>704</v>
       </c>
       <c r="H310">
-        <v>41085</v>
+        <v>41095</v>
       </c>
       <c r="I310">
-        <v>6580</v>
+        <v>6581</v>
       </c>
       <c r="J310" t="s">
         <v>745</v>
@@ -13808,10 +13808,10 @@
         <v>704</v>
       </c>
       <c r="H312">
-        <v>38181</v>
+        <v>38196</v>
       </c>
       <c r="I312">
-        <v>8544</v>
+        <v>8550</v>
       </c>
       <c r="J312" t="s">
         <v>753</v>
@@ -13843,10 +13843,10 @@
         <v>704</v>
       </c>
       <c r="H313">
-        <v>19325</v>
+        <v>19337</v>
       </c>
       <c r="I313">
-        <v>2231</v>
+        <v>2232</v>
       </c>
       <c r="J313" t="s">
         <v>745</v>
@@ -13913,10 +13913,10 @@
         <v>704</v>
       </c>
       <c r="H315">
-        <v>27022</v>
+        <v>27062</v>
       </c>
       <c r="I315">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="J315" t="s">
         <v>791</v>
@@ -14018,10 +14018,10 @@
         <v>702</v>
       </c>
       <c r="H318">
-        <v>63621</v>
+        <v>63630</v>
       </c>
       <c r="I318">
-        <v>16719</v>
+        <v>16721</v>
       </c>
       <c r="J318" t="s">
         <v>711</v>
@@ -14158,10 +14158,10 @@
         <v>704</v>
       </c>
       <c r="H322">
-        <v>74327</v>
+        <v>74333</v>
       </c>
       <c r="I322">
-        <v>8264</v>
+        <v>8265</v>
       </c>
       <c r="J322" t="s">
         <v>745</v>
@@ -14193,10 +14193,10 @@
         <v>704</v>
       </c>
       <c r="H323">
-        <v>28479</v>
+        <v>28483</v>
       </c>
       <c r="I323">
-        <v>6700</v>
+        <v>6702</v>
       </c>
       <c r="J323" t="s">
         <v>752</v>
@@ -14228,10 +14228,10 @@
         <v>704</v>
       </c>
       <c r="H324">
-        <v>35321</v>
+        <v>35324</v>
       </c>
       <c r="I324">
-        <v>5941</v>
+        <v>5943</v>
       </c>
       <c r="J324" t="s">
         <v>747</v>
@@ -14263,10 +14263,10 @@
         <v>704</v>
       </c>
       <c r="H325">
-        <v>52307</v>
+        <v>52314</v>
       </c>
       <c r="I325">
-        <v>10541</v>
+        <v>10542</v>
       </c>
       <c r="J325" t="s">
         <v>745</v>
@@ -14298,10 +14298,10 @@
         <v>702</v>
       </c>
       <c r="H326">
-        <v>185862</v>
+        <v>185934</v>
       </c>
       <c r="I326">
-        <v>15601</v>
+        <v>15608</v>
       </c>
       <c r="J326" t="s">
         <v>780</v>
@@ -14333,10 +14333,10 @@
         <v>704</v>
       </c>
       <c r="H327">
-        <v>85950</v>
+        <v>85976</v>
       </c>
       <c r="I327">
-        <v>7552</v>
+        <v>7553</v>
       </c>
       <c r="J327" t="s">
         <v>745</v>
@@ -14368,10 +14368,10 @@
         <v>704</v>
       </c>
       <c r="H328">
-        <v>59536</v>
+        <v>59540</v>
       </c>
       <c r="I328">
-        <v>15580</v>
+        <v>15583</v>
       </c>
       <c r="J328" t="s">
         <v>752</v>
@@ -14403,10 +14403,10 @@
         <v>704</v>
       </c>
       <c r="H329">
-        <v>145458</v>
+        <v>145602</v>
       </c>
       <c r="I329">
-        <v>18531</v>
+        <v>18542</v>
       </c>
       <c r="J329" t="s">
         <v>729</v>
@@ -14438,10 +14438,10 @@
         <v>702</v>
       </c>
       <c r="H330">
-        <v>109698</v>
+        <v>109721</v>
       </c>
       <c r="I330">
-        <v>31165</v>
+        <v>31171</v>
       </c>
       <c r="J330" t="s">
         <v>790</v>
@@ -14473,10 +14473,10 @@
         <v>704</v>
       </c>
       <c r="H331">
-        <v>454981</v>
+        <v>455064</v>
       </c>
       <c r="I331">
-        <v>66675</v>
+        <v>66694</v>
       </c>
       <c r="J331" t="s">
         <v>717</v>
@@ -14508,10 +14508,10 @@
         <v>704</v>
       </c>
       <c r="H332">
-        <v>123420</v>
+        <v>123441</v>
       </c>
       <c r="I332">
-        <v>54122</v>
+        <v>54137</v>
       </c>
       <c r="J332" t="s">
         <v>719</v>
@@ -14543,10 +14543,10 @@
         <v>704</v>
       </c>
       <c r="H333">
-        <v>327065</v>
+        <v>327097</v>
       </c>
       <c r="I333">
-        <v>32913</v>
+        <v>32926</v>
       </c>
       <c r="J333" t="s">
         <v>709</v>
@@ -14578,10 +14578,10 @@
         <v>702</v>
       </c>
       <c r="H334">
-        <v>468894</v>
+        <v>469035</v>
       </c>
       <c r="I334">
-        <v>58528</v>
+        <v>58547</v>
       </c>
       <c r="J334" t="s">
         <v>797</v>
@@ -14613,10 +14613,10 @@
         <v>702</v>
       </c>
       <c r="H335">
-        <v>281339</v>
+        <v>281429</v>
       </c>
       <c r="I335">
-        <v>101120</v>
+        <v>101149</v>
       </c>
       <c r="J335" t="s">
         <v>798</v>
@@ -14683,10 +14683,10 @@
         <v>702</v>
       </c>
       <c r="H337">
-        <v>384472</v>
+        <v>384576</v>
       </c>
       <c r="I337">
-        <v>39110</v>
+        <v>39121</v>
       </c>
       <c r="J337" t="s">
         <v>782</v>
@@ -14718,10 +14718,10 @@
         <v>704</v>
       </c>
       <c r="H338">
-        <v>238611</v>
+        <v>238646</v>
       </c>
       <c r="I338">
-        <v>55144</v>
+        <v>55162</v>
       </c>
       <c r="J338" t="s">
         <v>799</v>
@@ -14753,10 +14753,10 @@
         <v>702</v>
       </c>
       <c r="H339">
-        <v>317064</v>
+        <v>317180</v>
       </c>
       <c r="I339">
-        <v>112373</v>
+        <v>112415</v>
       </c>
       <c r="J339" t="s">
         <v>711</v>
@@ -14788,10 +14788,10 @@
         <v>704</v>
       </c>
       <c r="H340">
-        <v>720985</v>
+        <v>721127</v>
       </c>
       <c r="I340">
-        <v>195112</v>
+        <v>195181</v>
       </c>
       <c r="J340" t="s">
         <v>716</v>
@@ -14823,10 +14823,10 @@
         <v>702</v>
       </c>
       <c r="H341">
-        <v>171527</v>
+        <v>171549</v>
       </c>
       <c r="I341">
-        <v>40261</v>
+        <v>40274</v>
       </c>
       <c r="J341" t="s">
         <v>711</v>
@@ -14858,10 +14858,10 @@
         <v>704</v>
       </c>
       <c r="H342">
-        <v>431499</v>
+        <v>431540</v>
       </c>
       <c r="I342">
-        <v>59628</v>
+        <v>59638</v>
       </c>
       <c r="J342" t="s">
         <v>717</v>
@@ -14893,10 +14893,10 @@
         <v>706</v>
       </c>
       <c r="H343">
-        <v>291219</v>
+        <v>291244</v>
       </c>
       <c r="I343">
-        <v>62642</v>
+        <v>62651</v>
       </c>
       <c r="J343" t="s">
         <v>800</v>
@@ -14928,10 +14928,10 @@
         <v>704</v>
       </c>
       <c r="H344">
-        <v>328431</v>
+        <v>328529</v>
       </c>
       <c r="I344">
-        <v>59043</v>
+        <v>59062</v>
       </c>
       <c r="J344" t="s">
         <v>801</v>
@@ -14963,10 +14963,10 @@
         <v>704</v>
       </c>
       <c r="H345">
-        <v>188126</v>
+        <v>188177</v>
       </c>
       <c r="I345">
-        <v>69322</v>
+        <v>69356</v>
       </c>
       <c r="J345" t="s">
         <v>719</v>
@@ -14998,10 +14998,10 @@
         <v>704</v>
       </c>
       <c r="H346">
-        <v>317481</v>
+        <v>317543</v>
       </c>
       <c r="I346">
-        <v>117416</v>
+        <v>117448</v>
       </c>
       <c r="J346" t="s">
         <v>802</v>
@@ -15033,10 +15033,10 @@
         <v>704</v>
       </c>
       <c r="H347">
-        <v>508142</v>
+        <v>508238</v>
       </c>
       <c r="I347">
-        <v>143046</v>
+        <v>143086</v>
       </c>
       <c r="J347" t="s">
         <v>717</v>
@@ -15068,10 +15068,10 @@
         <v>704</v>
       </c>
       <c r="H348">
-        <v>283037</v>
+        <v>283118</v>
       </c>
       <c r="I348">
-        <v>127206</v>
+        <v>127262</v>
       </c>
       <c r="J348" t="s">
         <v>717</v>
@@ -15103,10 +15103,10 @@
         <v>704</v>
       </c>
       <c r="H349">
-        <v>399003</v>
+        <v>399054</v>
       </c>
       <c r="I349">
-        <v>103531</v>
+        <v>103554</v>
       </c>
       <c r="J349" t="s">
         <v>721</v>
@@ -15138,10 +15138,10 @@
         <v>702</v>
       </c>
       <c r="H350">
-        <v>565833</v>
+        <v>566011</v>
       </c>
       <c r="I350">
-        <v>234484</v>
+        <v>234559</v>
       </c>
       <c r="J350" t="s">
         <v>803</v>
@@ -15173,10 +15173,10 @@
         <v>703</v>
       </c>
       <c r="H351">
-        <v>6476022</v>
+        <v>6476640</v>
       </c>
       <c r="I351">
-        <v>5347828</v>
+        <v>5348264</v>
       </c>
       <c r="J351" t="s">
         <v>804</v>

</xml_diff>